<commit_message>
Auto-committed on 2022/02/15 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28EBA74-947F-4D7F-B6AD-92F6978296A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9542D83-0745-4D42-9973-1FF3433A7AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,24 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">User審查意見彙整!$A$1:$I$69</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="174">
   <si>
     <t>章節及說明</t>
   </si>
@@ -660,6 +653,288 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>修改後為不開放
+無法檢視是否不開放功能正常無誤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1001_顧客明細資料查詢
+此功能在L1001_顧客明細資料查詢，無法點選設定，選單也無此選項。只能直接用號碼才能變更。請修正，應於L1001_顧客明細資料查詢時，能直接點選功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">顯示畫面
+此按鈕應設立在共同位置，如最上方或最下方，如下圖
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>違約適用方式003依核准額度、004依申貸金額：
+文字意思是否有問題，
+3.自借款日起算，於未滿 36個月期間提前清償者，每次還款按核准額度，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取
+4.自借款日起算，於未滿 36個月期間提前清償者，每次還款依撥款金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>違約金分段月數：如何不分段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>違約適用方式：
+001綁約[按年分段]、002綁約[按月分段]、005依提前償還金額，有啥差異?
+1.自借款日起算，於未滿 36個月期間提前清償者，按各次提前清償金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取
+2.自借款日起算，於未滿 36個月期間提前清償者，按各次提前清償金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取
+5.自借款日起算，於未滿 36個月期間提前清償者，按各次提前清償金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加減碼是否依合約記號：要如何修改?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根據PJ201800012_URS_2業務作業_V1.5【L2001商品參數明細資料查詢】，所寫狀態有停用：
+怎麼停用?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄位【企金可使用記號】
+企金可使用記號，此功能為何?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PJ201800012_URS_2業務作業_V1.5，3.2_L2101商品參數維護：
+欄位【商品狀態】與【L2001商品參數明細資料查詢】，寫法不一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PJ201800012_URS_2業務作業_V1.5，3.2_L2101商品參數維護：
+未提及【企金可使用記號】，但系統畫面有此欄位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄位【生效日期】： 
+改_啟用日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄位【商品狀態】：停用，條件為何?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄位【商品狀態】：已生效，改_啟用
+未生效，改_未啟用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PJ201800012_URS_2業務作業_V1.5，P68，商品狀態，
+1:已生效
+2:未生效
+3:已截止
+4:停用：與畫面顯示不同</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄位【生效日期】：改_啟用日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欄位【企金可使用記號】：
+企金可使用記號，此功能為何?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">L2305借款戶關係人/關係企業維護(整批)         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2613法務費轉催收明細表                      </t>
+  </si>
+  <si>
+    <t>L2942法拍費用查詢-依會計日期</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5060案件處理清單         </t>
+  </si>
+  <si>
+    <t>L5062法務催收人員查詢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5601電催登錄             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5602面催登錄             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5603函催登錄             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5604法務進度登錄         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5605提醒事項登錄         </t>
+  </si>
+  <si>
+    <t>L5606法務催收人員維護</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5960案件資料查詢         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5961電催明細資料查詢     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5962面催明細資料查詢     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5963函催明細資料查詢     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5964法務進度明細資料查詢 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5965提醒事項查詢         </t>
+  </si>
+  <si>
+    <t>L6605逾期新增減少原因維護</t>
+  </si>
+  <si>
+    <t>L6987呆帳戶產生法務費墊付</t>
+  </si>
+  <si>
+    <t>L7022違約損失率檔查詢</t>
+  </si>
+  <si>
+    <t>L7202違約損失率登錄</t>
+  </si>
+  <si>
+    <t>L7204特殊客觀減損狀況維護</t>
+  </si>
+  <si>
+    <t>L7901３４號公報欄位清單產生作業</t>
+  </si>
+  <si>
+    <t>請演練(或說明)整批如何進行</t>
+  </si>
+  <si>
+    <t>新增測試資料後未顯示可轉催收明細</t>
+  </si>
+  <si>
+    <t>單據日期欄位移至收件日期之右</t>
+  </si>
+  <si>
+    <t>新增功能可列示於L6065畫面下方即可</t>
+  </si>
+  <si>
+    <t>增加戶況欄位(僅呆帳戶案件可顯示)</t>
+  </si>
+  <si>
+    <t>各類別最新資料新增『複製』功能</t>
+  </si>
+  <si>
+    <t>新增功能：『類別』 增加下拉選單合併『類別型態』為一個欄位</t>
+  </si>
+  <si>
+    <t>客觀減損條件增加下拉選單</t>
+  </si>
+  <si>
+    <t>張舜雯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查詢條件為1.2.3時，逾期數(天數)、戶況及地區為非必要輸入條件
+借款人身分證無法輸入統編(請增加法人欄位)
+查詢條件輸入5.6時地區別未輸入則顯示全部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.查詢條件為1.2.3時已調整,逾期數(天數)不輸入時預設為0,戶況預設為99全部,地區別預設為00全部
+2.經測試可正常輸入統編
+3.地區別一律預設為00全部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增複製功能,類別中文改以下拉式選單之中文帶入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>類別改為下拉式選單,預先建檔02~08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>檔案產生完成於LC009，但如何查看程式執行中還是異常？
+尚缺『五類資產分類上傳轉檔作業』</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增功能按鈕位置為統一位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地區別增加顯示中文,輸入條件增加法催人員姓名,若法催人員非空白則篩選條件增加法務人員或催收人員姓名相符之資料,增加員編條件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已電話聯絡告知測試方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客觀減損條件改為下拉式選單,預先建檔01~05,中文預設為客觀減損條件1~客觀減損條件5,待User確認中文敘述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.L6970批次執行結果查詢
+2.待確認作法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/2/11意見通過</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無案例無法進入該畫面檢測
+2022/2/11 接話人欄位出現錯誤訊息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無案例無法進入該畫面檢測；2022/2/11 『擔保品編號』應該為『擔保品地址』或是提供下拉選單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/2/8、2022/2/11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無案例無法進入該畫面檢測；2022/2/11 『擔保品編號』應該為『擔保品地址』或是提供下拉選單
+下行電文有誤:false-80801-TT101Session逾時或無效 請重新登入系統|</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無案例無法進入該畫面檢測；2022/2/11 項目預設:9 餘OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>除以『地區別』(應顯示中文)，應有『法催人員』(姓名)查詢.
+2022/2/11意見通過</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無案例無法進入該畫面檢測。2022/2/11意見通過</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請協助確認 人員修後案件是否同步完成修改？個案人員指派該如何處理？2022/2/11意見通過</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/11已電話聯絡告知測試方式
+2/14修改預設值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.程式調整為同步維護CollList之法務人員與催收人員
+2.個案人員指派功能,新增交易[L5607個案人員指派維護]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PJ201800012_URS_1顧客管理作業_V1.45，P10【2.[CustMain.ALWINQ開放查詢]欄位的處理邏輯：
 (1).不開放查詢客戶資料(需判斷登入者的單位別，單位別=0000總公司可以全查，若為分公司則只能查分公司建立的案件)只能看到帳務面資料:放款、案件、未齊件;不可以看到:顧客、電話、財報、保證人、擔保品、共同借款人、關聯戶、交互運用 
 (2).開放查詢客戶資料，全部人皆可查詢。】這段描述
@@ -668,285 +943,73 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>修改後為不開放
-無法檢視是否不開放功能正常無誤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>L1001_顧客明細資料查詢
-此功能在L1001_顧客明細資料查詢，無法點選設定，選單也無此選項。只能直接用號碼才能變更。請修正，應於L1001_顧客明細資料查詢時，能直接點選功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">顯示畫面
-此按鈕應設立在共同位置，如最上方或最下方，如下圖
+    <t>列入議題討論</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1001重新查詢後,"開放查詢"按鈕,會更新最新狀態為[開放]或[不開放]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前L1001查詢後,"開放查詢",會顯示狀態為[開放]或[不開放]按鈕供點選,不知問題為何?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系統共同設計
+1.新增按鈕置於查詢按鈕同列
+2.針對明細資料的功能鍵,會置於每筆資料同列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申請案件時案件隸屬單位為企金時可使用</t>
+  </si>
+  <si>
+    <t>無此欄位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不可修改 新商品預設Y</t>
+  </si>
+  <si>
+    <t>請說明</t>
+  </si>
+  <si>
+    <t>1.違約金分段月數輸入0為不分段
+2.不分段時,分段遞減百分比自動隱藏</t>
+  </si>
+  <si>
+    <t xml:space="preserve">需求規格書新增【企金可使用記號】欄位說明
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>違約適用方式003依核准額度、004依申貸金額：
-文字意思是否有問題，
-3.自借款日起算，於未滿 36個月期間提前清償者，每次還款按核准額度，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取
-4.自借款日起算，於未滿 36個月期間提前清償者，每次還款依撥款金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>違約金分段月數：如何不分段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>違約適用方式：
-001綁約[按年分段]、002綁約[按月分段]、005依提前償還金額，有啥差異?
-1.自借款日起算，於未滿 36個月期間提前清償者，按各次提前清償金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取
-2.自借款日起算，於未滿 36個月期間提前清償者，按各次提前清償金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取
-5.自借款日起算，於未滿 36個月期間提前清償者，按各次提前清償金額，1.00% 計付違約金，但每36個月遞減違約金1.00%，領清償證明時收取</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>加減碼是否依合約記號：要如何修改?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根據PJ201800012_URS_2業務作業_V1.5【L2001商品參數明細資料查詢】，所寫狀態有停用：
-怎麼停用?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄位【企金可使用記號】
-企金可使用記號，此功能為何?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PJ201800012_URS_2業務作業_V1.5，3.2_L2101商品參數維護：
-欄位【商品狀態】與【L2001商品參數明細資料查詢】，寫法不一致</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PJ201800012_URS_2業務作業_V1.5，3.2_L2101商品參數維護：
-未提及【企金可使用記號】，但系統畫面有此欄位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄位【生效日期】： 
-改_啟用日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄位【商品狀態】：停用，條件為何?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄位【商品狀態】：已生效，改_啟用
-未生效，改_未啟用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PJ201800012_URS_2業務作業_V1.5，P68，商品狀態，
+    <t xml:space="preserve">已更新欄位說明
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改URS文件與畫面一致
+0:全部
 1:已生效
-2:未生效
-3:已截止
-4:停用：與畫面顯示不同</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄位【生效日期】：改_啟用日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欄位【企金可使用記號】：
-企金可使用記號，此功能為何?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">L2305借款戶關係人/關係企業維護(整批)         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L2613法務費轉催收明細表                      </t>
-  </si>
-  <si>
-    <t>L2942法拍費用查詢-依會計日期</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5060案件處理清單         </t>
-  </si>
-  <si>
-    <t>L5062法務催收人員查詢</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5601電催登錄             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5602面催登錄             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5603函催登錄             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5604法務進度登錄         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5605提醒事項登錄         </t>
-  </si>
-  <si>
-    <t>L5606法務催收人員維護</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5960案件資料查詢         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5961電催明細資料查詢     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5962面催明細資料查詢     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5963函催明細資料查詢     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5964法務進度明細資料查詢 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L5965提醒事項查詢         </t>
-  </si>
-  <si>
-    <t>L6605逾期新增減少原因維護</t>
-  </si>
-  <si>
-    <t>L6987呆帳戶產生法務費墊付</t>
-  </si>
-  <si>
-    <t>L7022違約損失率檔查詢</t>
-  </si>
-  <si>
-    <t>L7202違約損失率登錄</t>
-  </si>
-  <si>
-    <t>L7204特殊客觀減損狀況維護</t>
-  </si>
-  <si>
-    <t>L7901３４號公報欄位清單產生作業</t>
-  </si>
-  <si>
-    <t>請演練(或說明)整批如何進行</t>
-  </si>
-  <si>
-    <t>新增測試資料後未顯示可轉催收明細</t>
-  </si>
-  <si>
-    <t>單據日期欄位移至收件日期之右</t>
-  </si>
-  <si>
-    <t>新增功能可列示於L6065畫面下方即可</t>
-  </si>
-  <si>
-    <t>增加戶況欄位(僅呆帳戶案件可顯示)</t>
-  </si>
-  <si>
-    <t>各類別最新資料新增『複製』功能</t>
-  </si>
-  <si>
-    <t>新增功能：『類別』 增加下拉選單合併『類別型態』為一個欄位</t>
-  </si>
-  <si>
-    <t>客觀減損條件增加下拉選單</t>
-  </si>
-  <si>
-    <t>張舜雯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查詢條件為1.2.3時，逾期數(天數)、戶況及地區為非必要輸入條件
-借款人身分證無法輸入統編(請增加法人欄位)
-查詢條件輸入5.6時地區別未輸入則顯示全部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.查詢條件為1.2.3時已調整,逾期數(天數)不輸入時預設為0,戶況預設為99全部,地區別預設為00全部
-2.經測試可正常輸入統編
-3.地區別一律預設為00全部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增複製功能,類別中文改以下拉式選單之中文帶入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>類別改為下拉式選單,預先建檔02~08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>檔案產生完成於LC009，但如何查看程式執行中還是異常？
-尚缺『五類資產分類上傳轉檔作業』</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增功能按鈕位置為統一位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地區別增加顯示中文,輸入條件增加法催人員姓名,若法催人員非空白則篩選條件增加法務人員或催收人員姓名相符之資料,增加員編條件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已電話聯絡告知測試方式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>客觀減損條件改為下拉式選單,預先建檔01~05,中文預設為客觀減損條件1~客觀減損條件5,待User確認中文敘述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.L6970批次執行結果查詢
-2.待確認作法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022/2/11意見通過</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>無案例無法進入該畫面檢測
-2022/2/11 接話人欄位出現錯誤訊息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>無案例無法進入該畫面檢測；2022/2/11 『擔保品編號』應該為『擔保品地址』或是提供下拉選單</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022/2/8、2022/2/11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>無案例無法進入該畫面檢測；2022/2/11 『擔保品編號』應該為『擔保品地址』或是提供下拉選單
-下行電文有誤:false-80801-TT101Session逾時或無效 請重新登入系統|</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>無案例無法進入該畫面檢測；2022/2/11 項目預設:9 餘OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>除以『地區別』(應顯示中文)，應有『法催人員』(姓名)查詢.
-2022/2/11意見通過</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>無案例無法進入該畫面檢測。2022/2/11意見通過</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>請協助確認 人員修後案件是否同步完成修改？個案人員指派該如何處理？2022/2/11意見通過</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2/11已電話聯絡告知測試方式
-2/14修改預設值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.程式調整為同步維護CollList之法務人員與催收人員
-2.個案人員指派功能,新增交易[L5607個案人員指派維護]</t>
+2:待生效
+3:已失效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">已更新文件說明,目前無停用選項
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前無停用選項,更新文件[商品狀態]欄位說明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[違約適用方式]為[001.綁約[按年分段]]時[違約分段月數]固定為12
+[違約適用方式]為[002.綁約[按月分段]]時[違約分段月數]需大於0
+[違約適用方式]為[005.依提前償還金額]時[違約分段月數]固定為0
+文件更新於PJ201800012_URS_2業務作業_V1.61
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -954,7 +1017,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1025,6 +1088,19 @@
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1113,7 +1189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1200,6 +1276,36 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1694,6 +1800,270 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22861</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>384210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4556761</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1196457</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="圖片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBD33A0C-D6F2-472D-B4D9-E4301DB0AC87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5532121" y="36259170"/>
+          <a:ext cx="4533900" cy="812247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4511409</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>884095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="圖片 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49EE97A8-247C-47B6-8ED6-7C55C0A8CF4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615940" y="37566600"/>
+          <a:ext cx="4404729" cy="655495"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1059180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4542025</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1781391</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="圖片 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9F2DA5-6A65-4348-BAD6-20BBBF679F79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5669280" y="38397180"/>
+          <a:ext cx="4382005" cy="722211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>106679</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2670406</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>2612402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="圖片 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{153ABA6C-01DF-4E29-A232-9DB67CDF8B01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615939" y="40005000"/>
+          <a:ext cx="2563727" cy="2338082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>2650444</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3886201</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>3219627</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="圖片 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B7D4970-09C6-4E6B-BEF0-80B2F460B240}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5623561" y="42381124"/>
+          <a:ext cx="3771900" cy="569183"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4427589</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>868855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="圖片 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7925555-A7FE-4F1A-A1BB-BDFB6326529F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5532120" y="34754820"/>
+          <a:ext cx="4404729" cy="655495"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1963,10 +2333,10 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F57" sqref="F57"/>
+      <selection pane="bottomRight" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2715,12 +3085,14 @@
         <v>82</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="E28" s="22">
         <v>44589</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2736,12 +3108,14 @@
         <v>82</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" s="22">
         <v>44589</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2757,12 +3131,14 @@
         <v>82</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" s="22">
         <v>44589</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2778,12 +3154,14 @@
         <v>83</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="22">
         <v>44589</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="7" t="s">
+        <v>162</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2799,12 +3177,14 @@
         <v>85</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E32" s="22">
         <v>44589</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="30" t="s">
+        <v>163</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2820,12 +3200,14 @@
         <v>85</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="22">
         <v>44589</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="32" t="s">
+        <v>164</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2841,12 +3223,14 @@
         <v>85</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E34" s="22">
         <v>44589</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="33" t="s">
+        <v>170</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2862,17 +3246,19 @@
         <v>85</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" s="22">
         <v>44589</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>84</v>
       </c>
@@ -2883,12 +3269,14 @@
         <v>85</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36" s="22">
         <v>44589</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="29" t="s">
+        <v>172</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2909,7 +3297,9 @@
       <c r="E37" s="22">
         <v>44589</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2925,17 +3315,19 @@
         <v>86</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E38" s="22">
         <v>44589</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>84</v>
       </c>
@@ -2946,17 +3338,19 @@
         <v>86</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E39" s="22">
         <v>44589</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="38" t="s">
+        <v>168</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>84</v>
       </c>
@@ -2967,12 +3361,14 @@
         <v>86</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E40" s="22">
         <v>44589</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="37" t="s">
+        <v>169</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -2988,17 +3384,19 @@
         <v>86</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E41" s="22">
         <v>44589</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="34" t="s">
+        <v>163</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="258" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
@@ -3009,12 +3407,14 @@
         <v>86</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E42" s="22">
         <v>44589</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="31" t="s">
+        <v>171</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -3030,12 +3430,14 @@
         <v>86</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E43" s="22">
         <v>44589</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="35" t="s">
+        <v>165</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -3051,12 +3453,14 @@
         <v>86</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E44" s="22">
         <v>44589</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="31" t="s">
+        <v>173</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -3072,12 +3476,14 @@
         <v>86</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E45" s="22">
         <v>44589</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="36" t="s">
+        <v>166</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -3093,28 +3499,30 @@
         <v>86</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E46" s="22">
         <v>44589</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="37" t="s">
+        <v>167</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="2">
         <v>1</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E47" s="22">
         <v>44600</v>
@@ -3126,16 +3534,16 @@
     </row>
     <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B48" s="2">
         <v>2</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E48" s="22">
         <v>44600</v>
@@ -3147,16 +3555,16 @@
     </row>
     <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B49" s="2">
         <v>3</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E49" s="22">
         <v>44600</v>
@@ -3168,22 +3576,22 @@
     </row>
     <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50" s="2">
         <v>4</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E50" s="22">
         <v>44600</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G50" s="15">
         <v>44601</v>
@@ -3195,22 +3603,22 @@
     </row>
     <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B51" s="2">
         <v>5</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E51" s="22">
         <v>44600</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G51" s="15">
         <v>44606</v>
@@ -3219,27 +3627,27 @@
         <v>67</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B52" s="2">
         <v>6</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G52" s="15">
         <v>44603</v>
@@ -3249,22 +3657,22 @@
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" s="2">
         <v>7</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E53" s="22">
         <v>44600</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G53" s="15">
         <v>44603</v>
@@ -3273,27 +3681,27 @@
         <v>67</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" s="2">
         <v>8</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E54" s="22">
         <v>44600</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G54" s="15">
         <v>44603</v>
@@ -3302,27 +3710,27 @@
         <v>67</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="2">
         <v>9</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E55" s="22" t="s">
-        <v>151</v>
-      </c>
       <c r="F55" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G55" s="15">
         <v>44603</v>
@@ -3332,22 +3740,22 @@
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B56" s="2">
         <v>10</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E56" s="22">
         <v>44600</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G56" s="15">
         <v>44603</v>
@@ -3356,54 +3764,54 @@
         <v>67</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B57" s="2">
         <v>11</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E57" s="22">
         <v>44600</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G57" s="15">
         <v>44603</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" s="2">
         <v>12</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G58" s="15">
         <v>44603</v>
@@ -3413,22 +3821,22 @@
     </row>
     <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="2">
         <v>13</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G59" s="15">
         <v>44606</v>
@@ -3440,22 +3848,22 @@
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" s="2">
         <v>14</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G60" s="15">
         <v>44606</v>
@@ -3467,22 +3875,22 @@
     </row>
     <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B61" s="2">
         <v>15</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G61" s="15">
         <v>44606</v>
@@ -3494,22 +3902,22 @@
     </row>
     <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B62" s="2">
         <v>16</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G62" s="15">
         <v>44606</v>
@@ -3521,22 +3929,22 @@
     </row>
     <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B63" s="2">
         <v>17</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E63" s="22">
         <v>44600</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G63" s="15">
         <v>44603</v>
@@ -3545,27 +3953,27 @@
         <v>67</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B64" s="2">
         <v>18</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E64" s="22">
         <v>44600</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G64" s="15">
         <v>44602</v>
@@ -3577,16 +3985,16 @@
     </row>
     <row r="65" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B65" s="2">
         <v>19</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E65" s="22">
         <v>44600</v>
@@ -3598,22 +4006,22 @@
     </row>
     <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B66" s="2">
         <v>20</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E66" s="22">
         <v>44600</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G66" s="15">
         <v>44601</v>
@@ -3625,22 +4033,22 @@
     </row>
     <row r="67" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B67" s="2">
         <v>21</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E67" s="22">
         <v>44600</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G67" s="15">
         <v>44601</v>
@@ -3652,22 +4060,22 @@
     </row>
     <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B68" s="2">
         <v>22</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E68" s="22">
         <v>44600</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G68" s="15">
         <v>44603</v>
@@ -3679,29 +4087,29 @@
     </row>
     <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B69" s="2">
         <v>23</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E69" s="22">
         <v>44600</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I69" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:I69" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="5" showButton="0"/>
     <filterColumn colId="6" showButton="0"/>
@@ -3718,21 +4126,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -3846,30 +4239,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3883,4 +4268,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/02/17 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF1268D-EBF0-4D5D-8876-E2FDA1C9C196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED4DE7D-F627-4D6E-A64E-7D72C531493C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="193">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1066,6 +1066,10 @@
   <si>
     <t>1.L6970批次執行結果查詢
 2.新增交易[L7205五類資產分類上傳轉檔作業]:月初時,月底日換日後夜間批次跑完的隔日下載LM051報表核對,若有錯誤則上傳五類資產分類檔案更新月報環境資料庫,重新產製LM051報表,確認無誤即可在月報環境執行L7901與L7902產生更新後的34號公報與IFRS9媒體檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多筆輸出畫面新增戶況欄位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3236,7 +3240,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{70159B45-7EE2-4047-BE71-D320E838B229}" name="樞紐分析表2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{70159B45-7EE2-4047-BE71-D320E838B229}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
   <location ref="A3:K12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -3711,11 +3715,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
+      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5455,8 +5459,12 @@
       <c r="E64" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F64" s="6"/>
-      <c r="G64" s="2"/>
+      <c r="F64" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G64" s="12">
+        <v>44608</v>
+      </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
@@ -6262,21 +6270,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -6390,17 +6383,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6414,17 +6423,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/02/21 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED4DE7D-F627-4D6E-A64E-7D72C531493C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A3A562-BCF0-4045-82DE-B94FC339F9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1064,12 +1064,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>多筆輸出畫面新增戶況欄位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.L6970批次執行結果查詢
-2.新增交易[L7205五類資產分類上傳轉檔作業]:月初時,月底日換日後夜間批次跑完的隔日下載LM051報表核對,若有錯誤則上傳五類資產分類檔案更新月報環境資料庫,重新產製LM051報表,確認無誤即可在月報環境執行L7901與L7902產生更新後的34號公報與IFRS9媒體檔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多筆輸出畫面新增戶況欄位</t>
+2.新增交易[L7205五類資產分類上傳轉檔作業]:月初時,月底日換日後夜間批次跑完的隔日下載LM051報表核對,若有錯誤則在月報環境上傳五類資產分類檔案更新月報環境資料庫,重新產製LM051報表,確認無誤即可在月報環境執行L7901與L7902產生更新後的34號公報與IFRS9媒體檔</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3719,7 +3719,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
+      <selection pane="bottomRight" activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5460,7 +5460,7 @@
         <v>142</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G64" s="12">
         <v>44608</v>
@@ -5566,7 +5566,7 @@
         <v>142</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G68" s="12">
         <v>44608</v>
@@ -6384,18 +6384,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6415,14 +6415,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -6435,4 +6427,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/02/25 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v06v2\Desktop\例會交付\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE41C7-F934-4987-86D8-1D1D16F6DC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA957AE9-A4BB-4394-9FA9-45D365CC23BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="79" r:id="rId3"/>
+    <pivotCache cacheId="77" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="195">
   <si>
     <t>章節及說明</t>
   </si>
@@ -2566,7 +2566,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44615.511249421295" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="66" xr:uid="{2BF1D914-C819-4B3D-AC98-E0D04F9116FB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44617.41105613426" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="66" xr:uid="{2BF1D914-C819-4B3D-AC98-E0D04F9116FB}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K67" sheet="User審查意見彙整"/>
   </cacheSource>
@@ -2792,8 +2792,8 @@
     <s v="是否比照[L2614法務費轉催收傳票開立作業(列印)]做法，請確認_x000a__x000a__x000a__x000a__x000a__x000a_"/>
     <d v="2022-01-21T00:00:00"/>
     <d v="2022-01-21T00:00:00"/>
+    <m/>
     <s v="待User確認"/>
-    <s v="無"/>
     <m/>
   </r>
   <r>
@@ -3468,7 +3468,7 @@
     <s v="客觀減損條件改為下拉式選單,預先建檔01~05,中文預設為客觀減損條件1~客觀減損條件5,待User確認中文敘述"/>
     <d v="2022-02-15T00:00:00"/>
     <d v="2022-02-11T00:00:00"/>
-    <m/>
+    <s v="已完成"/>
     <s v="待User確認"/>
     <m/>
   </r>
@@ -3481,7 +3481,7 @@
     <s v="1.L6970批次執行結果查詢_x000a_2.新增交易[L7205五類資產分類上傳轉檔作業]:月初時,月底日換日後夜間批次跑完的隔日下載LM051報表核對,若須調整則連線上傳五類資產分類檔案更新月報環境資料庫,重新產製LM051報表,即可在月報環境執行L7901與L7902產生更新後的34號公報與IFRS9媒體檔"/>
     <s v="2022/2/25_x000a_DEV_online測試環境完成始可測試。(2022/2/22~2/23)"/>
     <d v="2022-02-16T00:00:00"/>
-    <m/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3489,7 +3489,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{70159B45-7EE2-4047-BE71-D320E838B229}" name="樞紐分析表2" cacheId="79" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{70159B45-7EE2-4047-BE71-D320E838B229}" name="樞紐分析表2" cacheId="77" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
   <location ref="A3:K12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
@@ -3966,11 +3966,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
@@ -4445,11 +4445,8 @@
       <c r="H14" s="7">
         <v>44582</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>194</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -6167,6 +6164,9 @@
       <c r="H66" s="12">
         <v>44603</v>
       </c>
+      <c r="I66" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J66" s="7" t="s">
         <v>61</v>
       </c>
@@ -6197,7 +6197,9 @@
       <c r="H67" s="12">
         <v>44608</v>
       </c>
-      <c r="I67" s="7"/>
+      <c r="I67" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J67" s="7"/>
       <c r="K67" s="2"/>
     </row>
@@ -6214,8 +6216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC86E09E-B021-4224-A1E5-A5F4EAB63232}">
   <dimension ref="A3:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -6325,7 +6327,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="31">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
@@ -6335,7 +6337,7 @@
         <v>14</v>
       </c>
       <c r="K7" s="31">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -6369,7 +6371,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="31">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
@@ -6381,7 +6383,7 @@
         <v>23</v>
       </c>
       <c r="K9" s="31">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
@@ -6438,13 +6440,13 @@
         <v>23</v>
       </c>
       <c r="C12" s="31">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D12" s="31">
         <v>21</v>
       </c>
       <c r="E12" s="31">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="31">
         <v>3</v>
@@ -6462,7 +6464,7 @@
         <v>66</v>
       </c>
       <c r="K12" s="31">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.4">
@@ -6602,7 +6604,7 @@
       </c>
       <c r="C22" s="26">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="26">
         <f t="shared" si="0"/>
@@ -6634,11 +6636,11 @@
       </c>
       <c r="K22" s="29">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L22" s="35">
         <f t="shared" ref="L22:L27" si="10">K22/J22</f>
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
@@ -6726,7 +6728,7 @@
       </c>
       <c r="I24" s="26">
         <f>C9-1</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J24" s="29">
         <f t="shared" si="8"/>
@@ -6734,11 +6736,11 @@
       </c>
       <c r="K24" s="29">
         <f>K9-1</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L24" s="35">
         <f t="shared" si="10"/>
-        <v>0.86956521739130432</v>
+        <v>0.95652173913043481</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
@@ -6852,7 +6854,7 @@
       </c>
       <c r="C27" s="36">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" s="36">
         <f t="shared" si="0"/>
@@ -6876,19 +6878,19 @@
       </c>
       <c r="I27" s="36">
         <f>C12-1</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J27" s="42">
         <f t="shared" si="8"/>
         <v>66</v>
       </c>
       <c r="K27" s="42">
-        <f>K12-1</f>
-        <v>63</v>
+        <f>K12</f>
+        <v>65</v>
       </c>
       <c r="L27" s="43">
         <f t="shared" si="10"/>
-        <v>0.95454545454545459</v>
+        <v>0.98484848484848486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/11 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E5C58D-80CC-48F6-9EBA-A4D357621167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7205A7B4-9DDB-4189-BA49-3CE4CDB45A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="45" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -649,9 +649,6 @@
     <t>L7901３４號公報欄位清單產生作業</t>
   </si>
   <si>
-    <t>請演練(或說明)整批如何進行</t>
-  </si>
-  <si>
     <t>新增測試資料後未顯示可轉催收明細</t>
   </si>
   <si>
@@ -1091,6 +1088,10 @@
   </si>
   <si>
     <t>計數 - 意見收到日</t>
+  </si>
+  <si>
+    <t>請演練(或說明)整批如何進行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1387,833 +1388,7 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="126">
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="標楷體"/>
-        <family val="4"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <name val="標楷體"/>
@@ -4361,7 +3536,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB8491D-910A-4350-9E7C-5C300AE8C9CA}" name="樞紐分析表2" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB8491D-910A-4350-9E7C-5C300AE8C9CA}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0">
@@ -4434,28 +3609,28 @@
     <dataField name="回覆" fld="8" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="125">
+    <format dxfId="7">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="124">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="123">
+    <format dxfId="5">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="4">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="3">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="2">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="119">
+    <format dxfId="1">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="118">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -4736,47 +3911,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79:G85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6328125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="13" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="67.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>36</v>
@@ -4785,13 +3960,13 @@
         <v>59</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4820,11 +3995,11 @@
         <v>60</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -4853,11 +4028,11 @@
         <v>60</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4886,11 +4061,11 @@
         <v>60</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -4919,11 +4094,11 @@
         <v>60</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4952,11 +4127,11 @@
         <v>60</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4985,11 +4160,11 @@
         <v>60</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -5018,11 +4193,11 @@
         <v>60</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -5051,11 +4226,11 @@
         <v>60</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -5084,11 +4259,11 @@
         <v>60</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -5117,11 +4292,11 @@
         <v>60</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -5150,11 +4325,11 @@
         <v>60</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -5183,11 +4358,11 @@
         <v>60</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -5213,14 +4388,14 @@
         <v>44582</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>61</v>
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -5249,11 +4424,11 @@
         <v>60</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -5282,11 +4457,11 @@
         <v>60</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -5315,11 +4490,11 @@
         <v>60</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -5348,11 +4523,11 @@
         <v>60</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -5381,11 +4556,11 @@
         <v>60</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -5414,11 +4589,11 @@
         <v>60</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -5447,11 +4622,11 @@
         <v>60</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5480,11 +4655,11 @@
         <v>60</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5513,11 +4688,11 @@
         <v>60</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="246.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="255" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5546,11 +4721,11 @@
         <v>60</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5579,11 +4754,11 @@
         <v>60</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5594,13 +4769,13 @@
         <v>72</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" s="13">
         <v>44589</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G26" s="14">
         <v>44603</v>
@@ -5612,11 +4787,11 @@
         <v>60</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5633,7 +4808,7 @@
         <v>44589</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G27" s="14">
         <v>44603</v>
@@ -5645,11 +4820,11 @@
         <v>60</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -5666,7 +4841,7 @@
         <v>44589</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G28" s="14">
         <v>44603</v>
@@ -5678,11 +4853,11 @@
         <v>60</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -5699,7 +4874,7 @@
         <v>44589</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G29" s="14">
         <v>44603</v>
@@ -5711,11 +4886,11 @@
         <v>60</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -5732,7 +4907,7 @@
         <v>44589</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G30" s="14">
         <v>44603</v>
@@ -5741,14 +4916,14 @@
         <v>44607</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -5765,7 +4940,7 @@
         <v>44589</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G31" s="14">
         <v>44603</v>
@@ -5774,14 +4949,14 @@
         <v>44607</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="87" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -5798,7 +4973,7 @@
         <v>44589</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G32" s="14">
         <v>44603</v>
@@ -5807,14 +4982,14 @@
         <v>44607</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -5831,7 +5006,7 @@
         <v>44589</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G33" s="14">
         <v>44603</v>
@@ -5840,14 +5015,14 @@
         <v>44607</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -5864,7 +5039,7 @@
         <v>44589</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G34" s="14">
         <v>44603</v>
@@ -5873,14 +5048,14 @@
         <v>44607</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -5897,7 +5072,7 @@
         <v>44589</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G35" s="14">
         <v>44603</v>
@@ -5906,14 +5081,14 @@
         <v>44607</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -5930,7 +5105,7 @@
         <v>44589</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G36" s="14">
         <v>44603</v>
@@ -5939,14 +5114,14 @@
         <v>44607</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5963,7 +5138,7 @@
         <v>44589</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G37" s="14">
         <v>44603</v>
@@ -5972,14 +5147,14 @@
         <v>44607</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5996,7 +5171,7 @@
         <v>44589</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G38" s="13">
         <v>44603</v>
@@ -6005,14 +5180,14 @@
         <v>44607</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -6029,7 +5204,7 @@
         <v>44589</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G39" s="37">
         <v>44603</v>
@@ -6038,14 +5213,14 @@
         <v>44607</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -6062,7 +5237,7 @@
         <v>44589</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G40" s="38">
         <v>44603</v>
@@ -6071,14 +5246,14 @@
         <v>44607</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -6095,7 +5270,7 @@
         <v>44589</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G41" s="13">
         <v>44603</v>
@@ -6104,14 +5279,14 @@
         <v>44607</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="174" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -6128,7 +5303,7 @@
         <v>44589</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G42" s="38">
         <v>44603</v>
@@ -6140,11 +5315,11 @@
         <v>60</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -6161,7 +5336,7 @@
         <v>44589</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G43" s="13">
         <v>44603</v>
@@ -6170,14 +5345,14 @@
         <v>44607</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -6194,7 +5369,7 @@
         <v>44589</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G44" s="13">
         <v>44603</v>
@@ -6203,16 +5378,16 @@
         <v>44607</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="304.5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" ht="315" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" s="2">
         <v>1</v>
@@ -6221,13 +5396,13 @@
         <v>95</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>118</v>
+        <v>213</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G45" s="13">
         <v>44607</v>
@@ -6239,13 +5414,13 @@
         <v>60</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B46" s="2">
         <v>2</v>
@@ -6254,13 +5429,13 @@
         <v>96</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G46" s="13">
         <v>44607</v>
@@ -6272,13 +5447,13 @@
         <v>60</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B47" s="2">
         <v>3</v>
@@ -6287,13 +5462,13 @@
         <v>97</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G47" s="13">
         <v>44607</v>
@@ -6305,13 +5480,13 @@
         <v>60</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B48" s="2">
         <v>4</v>
@@ -6320,13 +5495,13 @@
         <v>98</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="G48" s="13">
         <v>44607</v>
@@ -6338,13 +5513,13 @@
         <v>60</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B49" s="2">
         <v>5</v>
@@ -6353,13 +5528,13 @@
         <v>99</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G49" s="13">
         <v>44607</v>
@@ -6371,15 +5546,15 @@
         <v>60</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B50" s="2">
         <v>6</v>
@@ -6388,13 +5563,13 @@
         <v>100</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G50" s="13">
         <v>44607</v>
@@ -6406,13 +5581,13 @@
         <v>60</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B51" s="2">
         <v>7</v>
@@ -6421,13 +5596,13 @@
         <v>101</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G51" s="13">
         <v>44607</v>
@@ -6439,15 +5614,15 @@
         <v>60</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="2">
         <v>8</v>
@@ -6456,13 +5631,13 @@
         <v>102</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G52" s="13">
         <v>44607</v>
@@ -6474,15 +5649,15 @@
         <v>60</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="2">
         <v>9</v>
@@ -6491,13 +5666,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>139</v>
-      </c>
       <c r="F53" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G53" s="13">
         <v>44607</v>
@@ -6509,13 +5684,13 @@
         <v>60</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B54" s="2">
         <v>10</v>
@@ -6524,13 +5699,13 @@
         <v>104</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G54" s="13">
         <v>44607</v>
@@ -6542,15 +5717,15 @@
         <v>60</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" s="2">
         <v>11</v>
@@ -6559,13 +5734,13 @@
         <v>105</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G55" s="13">
         <v>44607</v>
@@ -6577,13 +5752,13 @@
         <v>60</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B56" s="2">
         <v>12</v>
@@ -6592,13 +5767,13 @@
         <v>106</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G56" s="13">
         <v>44607</v>
@@ -6610,13 +5785,13 @@
         <v>60</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="2">
         <v>13</v>
@@ -6625,13 +5800,13 @@
         <v>107</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G57" s="13">
         <v>44607</v>
@@ -6643,13 +5818,13 @@
         <v>60</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="2">
         <v>14</v>
@@ -6658,13 +5833,13 @@
         <v>108</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G58" s="13">
         <v>44607</v>
@@ -6676,13 +5851,13 @@
         <v>60</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="2">
         <v>15</v>
@@ -6691,13 +5866,13 @@
         <v>109</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G59" s="13">
         <v>44607</v>
@@ -6709,13 +5884,13 @@
         <v>60</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="2">
         <v>16</v>
@@ -6724,13 +5899,13 @@
         <v>110</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G60" s="13">
         <v>44607</v>
@@ -6742,13 +5917,13 @@
         <v>60</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B61" s="2">
         <v>17</v>
@@ -6757,13 +5932,13 @@
         <v>111</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G61" s="13">
         <v>44607</v>
@@ -6775,15 +5950,15 @@
         <v>60</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B62" s="2">
         <v>18</v>
@@ -6792,13 +5967,13 @@
         <v>112</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G62" s="13">
         <v>44607</v>
@@ -6810,13 +5985,13 @@
         <v>60</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B63" s="2">
         <v>19</v>
@@ -6825,13 +6000,13 @@
         <v>113</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G63" s="13">
         <v>44607</v>
@@ -6843,13 +6018,13 @@
         <v>60</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" s="2">
         <v>20</v>
@@ -6858,13 +6033,13 @@
         <v>114</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G64" s="13">
         <v>44607</v>
@@ -6876,13 +6051,13 @@
         <v>60</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" s="2">
         <v>21</v>
@@ -6891,13 +6066,13 @@
         <v>115</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G65" s="13">
         <v>44607</v>
@@ -6909,13 +6084,13 @@
         <v>60</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B66" s="2">
         <v>22</v>
@@ -6924,13 +6099,13 @@
         <v>116</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G66" s="13">
         <v>44607</v>
@@ -6939,16 +6114,16 @@
         <v>44603</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J66" s="7" t="s">
         <v>61</v>
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="2">
         <v>23</v>
@@ -6957,16 +6132,16 @@
         <v>117</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F67" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G67" s="13" t="s">
         <v>182</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>183</v>
       </c>
       <c r="H67" s="11">
         <v>44608</v>
@@ -6975,22 +6150,22 @@
         <v>60</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B68" s="2">
         <v>1</v>
       </c>
       <c r="C68" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="E68" s="13">
         <v>44615</v>
@@ -7002,15 +6177,15 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B69" s="2">
         <v>2</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>93</v>
@@ -7025,18 +6200,18 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B70" s="2">
         <v>3</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E70" s="13">
         <v>44615</v>
@@ -7048,15 +6223,15 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B71" s="2">
         <v>4</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>91</v>
@@ -7071,15 +6246,15 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B72" s="2">
         <v>5</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>90</v>
@@ -7094,18 +6269,18 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B73" s="2">
         <v>6</v>
       </c>
       <c r="C73" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="E73" s="13">
         <v>44615</v>
@@ -7117,18 +6292,18 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B74" s="2">
         <v>7</v>
       </c>
       <c r="C74" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="E74" s="13">
         <v>44615</v>
@@ -7140,18 +6315,18 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B75" s="2">
         <v>8</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E75" s="13">
         <v>44615</v>
@@ -7163,18 +6338,18 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B76" s="2">
         <v>9</v>
       </c>
       <c r="C76" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="E76" s="13">
         <v>44615</v>
@@ -7186,18 +6361,18 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B77" s="2">
         <v>10</v>
       </c>
       <c r="C77" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="E77" s="13">
         <v>44615</v>
@@ -7209,185 +6384,201 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B78" s="2">
         <v>11</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E78" s="13">
         <v>44615</v>
       </c>
       <c r="F78" s="2"/>
-      <c r="G78" s="14"/>
+      <c r="G78" s="14">
+        <v>44636</v>
+      </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B79" s="2">
         <v>12</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E79" s="13">
         <v>44615</v>
       </c>
       <c r="F79" s="2"/>
-      <c r="G79" s="14"/>
+      <c r="G79" s="14">
+        <v>44636</v>
+      </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B80" s="2">
         <v>13</v>
       </c>
       <c r="C80" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="E80" s="13">
         <v>44615</v>
       </c>
       <c r="F80" s="2"/>
-      <c r="G80" s="14"/>
+      <c r="G80" s="14">
+        <v>44636</v>
+      </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" s="2">
         <v>14</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E81" s="13">
         <v>44615</v>
       </c>
       <c r="F81" s="2"/>
-      <c r="G81" s="14"/>
+      <c r="G81" s="14">
+        <v>44636</v>
+      </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B82" s="2">
         <v>15</v>
       </c>
       <c r="C82" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D82" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="E82" s="13">
         <v>44615</v>
       </c>
       <c r="F82" s="2"/>
-      <c r="G82" s="14"/>
+      <c r="G82" s="14">
+        <v>44636</v>
+      </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B83" s="2">
         <v>16</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E83" s="13">
         <v>44615</v>
       </c>
       <c r="F83" s="2"/>
-      <c r="G83" s="14"/>
+      <c r="G83" s="14">
+        <v>44636</v>
+      </c>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" s="2">
         <v>17</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E84" s="13">
         <v>44615</v>
       </c>
       <c r="F84" s="2"/>
-      <c r="G84" s="14"/>
+      <c r="G84" s="14">
+        <v>44636</v>
+      </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B85" s="2">
         <v>18</v>
       </c>
       <c r="C85" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D85" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="E85" s="13">
         <v>44615</v>
       </c>
       <c r="F85" s="2"/>
-      <c r="G85" s="14"/>
+      <c r="G85" s="14">
+        <v>44636</v>
+      </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
@@ -7410,33 +6601,33 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="17"/>
+    <col min="12" max="12" width="14.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="17"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -7449,9 +6640,9 @@
       <c r="L3"/>
       <c r="M3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="22">
         <v>23</v>
@@ -7470,7 +6661,7 @@
       <c r="L4"/>
       <c r="M4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="42">
         <v>44575</v>
       </c>
@@ -7491,7 +6682,7 @@
       <c r="L5"/>
       <c r="M5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="42">
         <v>44587</v>
       </c>
@@ -7512,7 +6703,7 @@
       <c r="L6"/>
       <c r="M6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="42">
         <v>44589</v>
       </c>
@@ -7533,7 +6724,7 @@
       <c r="L7"/>
       <c r="M7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="42">
         <v>44615</v>
       </c>
@@ -7552,9 +6743,9 @@
       <c r="L8"/>
       <c r="M8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="22">
         <v>84</v>
@@ -7573,7 +6764,7 @@
       <c r="L9"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -7588,7 +6779,7 @@
       <c r="L10"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -7603,7 +6794,7 @@
       <c r="L11"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -7618,27 +6809,27 @@
       <c r="L12"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
     </row>
-    <row r="19" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="str">
         <f>B3</f>
         <v>計數 - 意見收到日</v>
@@ -7658,16 +6849,16 @@
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I19" s="29"/>
       <c r="J19" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K19" s="31"/>
       <c r="L19" s="32"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="27">
         <f t="shared" ref="A20" si="2">A5</f>
         <v>44575</v>
@@ -7705,16 +6896,16 @@
         <v>21</v>
       </c>
       <c r="J20" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K20" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L20" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <f t="shared" ref="A21" si="7">A6</f>
         <v>44587</v>
@@ -7764,7 +6955,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="17">
         <f t="shared" ref="A22" si="9">A7</f>
         <v>44589</v>
@@ -7814,7 +7005,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <f t="shared" ref="A23" si="11">A8</f>
         <v>44615</v>
@@ -7864,7 +7055,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="str">
         <f t="shared" ref="A24" si="12">A9</f>
         <v>總計</v>
@@ -7914,7 +7105,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <f t="shared" ref="A25" si="13">A10</f>
         <v>0</v>
@@ -7964,7 +7155,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <f t="shared" ref="A26" si="14">A11</f>
         <v>0</v>
@@ -8014,7 +7205,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <f t="shared" ref="A27" si="15">A12</f>
         <v>0</v>
@@ -8071,6 +7262,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -8184,33 +7390,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8231,9 +7414,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/14 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B93E2E-774C-427E-9326-E44C12C3BF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1480DD5-B3DA-46BA-97ED-48B842AE6EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="220">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1090,6 +1090,26 @@
   </si>
   <si>
     <t>L2631不檢查須由入口交易進入 可由選單點擊進入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原為預設日期，可不輸入，已經預設部分移除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原為因實際還款日有值(自動帶入)則金額必須輸入，現實際還款日不自動帶入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加查詢按鈕供查看資料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>僅供依此條件查看延遲交易確認資料，若需移除條件也可以</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UAT環境，可查詢入帳日期=1101229</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3535,7 +3555,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB8491D-910A-4350-9E7C-5C300AE8C9CA}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB8491D-910A-4350-9E7C-5C300AE8C9CA}" name="樞紐分析表2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0">
@@ -3910,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -6354,9 +6374,15 @@
       <c r="E75" s="13">
         <v>44615</v>
       </c>
-      <c r="F75" s="2"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="2"/>
+      <c r="F75" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G75" s="14">
+        <v>44636</v>
+      </c>
+      <c r="H75" s="11">
+        <v>44634</v>
+      </c>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
@@ -6377,11 +6403,15 @@
       <c r="E76" s="13">
         <v>44615</v>
       </c>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="G76" s="14">
         <v>44636</v>
       </c>
-      <c r="H76" s="2"/>
+      <c r="H76" s="11">
+        <v>44634</v>
+      </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -6402,11 +6432,15 @@
       <c r="E77" s="13">
         <v>44615</v>
       </c>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="G77" s="14">
         <v>44636</v>
       </c>
-      <c r="H77" s="2"/>
+      <c r="H77" s="11">
+        <v>44634</v>
+      </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -6427,11 +6461,15 @@
       <c r="E78" s="13">
         <v>44615</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="G78" s="14">
         <v>44636</v>
       </c>
-      <c r="H78" s="2"/>
+      <c r="H78" s="11">
+        <v>44634</v>
+      </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -6452,11 +6490,15 @@
       <c r="E79" s="13">
         <v>44615</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="10" t="s">
+        <v>218</v>
+      </c>
       <c r="G79" s="14">
         <v>44636</v>
       </c>
-      <c r="H79" s="2"/>
+      <c r="H79" s="11">
+        <v>44634</v>
+      </c>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -6477,11 +6519,15 @@
       <c r="E80" s="13">
         <v>44615</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="G80" s="14">
         <v>44636</v>
       </c>
-      <c r="H80" s="2"/>
+      <c r="H80" s="11">
+        <v>44634</v>
+      </c>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -6502,11 +6548,15 @@
       <c r="E81" s="13">
         <v>44615</v>
       </c>
-      <c r="F81" s="2"/>
+      <c r="F81" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="G81" s="14">
         <v>44636</v>
       </c>
-      <c r="H81" s="2"/>
+      <c r="H81" s="11">
+        <v>44634</v>
+      </c>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
@@ -6527,11 +6577,15 @@
       <c r="E82" s="13">
         <v>44615</v>
       </c>
-      <c r="F82" s="2"/>
+      <c r="F82" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="G82" s="14">
         <v>44636</v>
       </c>
-      <c r="H82" s="2"/>
+      <c r="H82" s="11">
+        <v>44634</v>
+      </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -6552,11 +6606,15 @@
       <c r="E83" s="13">
         <v>44615</v>
       </c>
-      <c r="F83" s="2"/>
+      <c r="F83" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="G83" s="14">
         <v>44636</v>
       </c>
-      <c r="H83" s="2"/>
+      <c r="H83" s="11">
+        <v>44634</v>
+      </c>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -7239,21 +7297,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -7367,17 +7410,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7391,17 +7450,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/15 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1480DD5-B3DA-46BA-97ED-48B842AE6EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE06B59-45CE-40E9-9D41-DEA4527C6441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="224">
   <si>
     <t>章節及說明</t>
   </si>
@@ -961,9 +961,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>無符合結案區分之撥款資料，無法執行</t>
-  </si>
-  <si>
     <t>L2632清償作業維護</t>
   </si>
   <si>
@@ -1110,6 +1107,26 @@
   </si>
   <si>
     <t>UAT環境，可查詢入帳日期=1101229</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2631新增清償資料後,再次L2077查詢點【修改】【刪除】按鈕進入L2632維護</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無符合結案區分之撥款資料，無法執行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>檢查此戶號是否有符合結案區分資料,若無則顯示錯誤訊息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已做L2631新增清償資料並執行L3420結案登錄後,L2077顯示按鈕可連動至L2076</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶號改為區間查詢</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3555,7 +3572,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB8491D-910A-4350-9E7C-5C300AE8C9CA}" name="樞紐分析表2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3AB8491D-910A-4350-9E7C-5C300AE8C9CA}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="User" colHeaderCaption="意見收到日">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0">
@@ -3930,8 +3947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3961,13 +3978,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G1" s="36" t="s">
         <v>180</v>
@@ -4407,7 +4424,7 @@
         <v>44582</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>61</v>
@@ -5355,7 +5372,7 @@
         <v>44589</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G43" s="13">
         <v>44603</v>
@@ -5415,7 +5432,7 @@
         <v>95</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>138</v>
@@ -6133,7 +6150,7 @@
         <v>44603</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J66" s="7" t="s">
         <v>61</v>
@@ -6189,8 +6206,12 @@
       <c r="E68" s="13">
         <v>44615</v>
       </c>
-      <c r="F68" s="2"/>
-      <c r="G68" s="14"/>
+      <c r="F68" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G68" s="14">
+        <v>44642</v>
+      </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
@@ -6213,7 +6234,7 @@
         <v>44615</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G69" s="14">
         <v>44631</v>
@@ -6244,7 +6265,7 @@
         <v>44615</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G70" s="14">
         <v>44631</v>
@@ -6274,10 +6295,18 @@
       <c r="E71" s="13">
         <v>44615</v>
       </c>
-      <c r="F71" s="2"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
+      <c r="F71" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G71" s="14">
+        <v>44635</v>
+      </c>
+      <c r="H71" s="14">
+        <v>44635</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
@@ -6298,7 +6327,7 @@
         <v>44615</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G72" s="14">
         <v>44631</v>
@@ -6323,15 +6352,23 @@
         <v>189</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>191</v>
+        <v>220</v>
       </c>
       <c r="E73" s="13">
         <v>44615</v>
       </c>
-      <c r="F73" s="2"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
+      <c r="F73" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G73" s="14">
+        <v>44635</v>
+      </c>
+      <c r="H73" s="14">
+        <v>44635</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
@@ -6343,18 +6380,26 @@
         <v>9</v>
       </c>
       <c r="C74" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="E74" s="13">
         <v>44615</v>
       </c>
-      <c r="F74" s="2"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
+      <c r="F74" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G74" s="14">
+        <v>44635</v>
+      </c>
+      <c r="H74" s="14">
+        <v>44635</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
@@ -6366,16 +6411,16 @@
         <v>10</v>
       </c>
       <c r="C75" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D75" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="E75" s="13">
         <v>44615</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G75" s="14">
         <v>44636</v>
@@ -6395,16 +6440,16 @@
         <v>11</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E76" s="13">
         <v>44615</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G76" s="14">
         <v>44636</v>
@@ -6424,16 +6469,16 @@
         <v>12</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E77" s="13">
         <v>44615</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G77" s="14">
         <v>44636</v>
@@ -6453,16 +6498,16 @@
         <v>13</v>
       </c>
       <c r="C78" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="E78" s="13">
         <v>44615</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G78" s="14">
         <v>44636</v>
@@ -6482,16 +6527,16 @@
         <v>14</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E79" s="13">
         <v>44615</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G79" s="14">
         <v>44636</v>
@@ -6511,16 +6556,16 @@
         <v>15</v>
       </c>
       <c r="C80" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="E80" s="13">
         <v>44615</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G80" s="14">
         <v>44636</v>
@@ -6540,16 +6585,16 @@
         <v>16</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E81" s="13">
         <v>44615</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G81" s="14">
         <v>44636</v>
@@ -6569,16 +6614,16 @@
         <v>17</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E82" s="13">
         <v>44615</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G82" s="14">
         <v>44636</v>
@@ -6598,16 +6643,16 @@
         <v>18</v>
       </c>
       <c r="C83" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D83" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="E83" s="13">
         <v>44615</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G83" s="14">
         <v>44636</v>
@@ -6659,7 +6704,7 @@
         <v>173</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>171</v>
@@ -7297,6 +7342,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -7410,22 +7470,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7439,27 +7507,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/21 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDAF84C-1A27-44C2-A23C-3F2DBC9C8431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95015539-EE65-4CC9-8D85-D9FD1CC0C1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="1488" yWindow="0" windowWidth="19620" windowHeight="11856" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="253">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1208,6 +1208,31 @@
   </si>
   <si>
     <t>2022/2/8、11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>程慧娟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.授權辦理事項：三個選項應為■查詢■覆核■其他，請將系統第一個選項審查更改為查詢。
+2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L8950、L8350、L8351</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>銷號欄開放輸入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有判斷此額度已全部結清才可領取清償證明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已修正</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2411,15 +2436,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1727200</xdr:colOff>
+          <xdr:colOff>1729740</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>50800</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2216150</xdr:colOff>
+          <xdr:colOff>2217420</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>330200</xdr:rowOff>
+          <xdr:rowOff>327660</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2466,15 +2491,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2311400</xdr:colOff>
+          <xdr:colOff>2308860</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>222250</xdr:rowOff>
+          <xdr:rowOff>220980</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>2933700</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>539750</xdr:rowOff>
+          <xdr:rowOff>541020</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3808,7 +3833,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:S12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -4223,31 +4248,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6328125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="67.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>162</v>
       </c>
@@ -4282,7 +4307,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4315,7 +4340,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -4348,7 +4373,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4381,7 +4406,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -4414,7 +4439,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4447,7 +4472,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4480,7 +4505,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4513,7 +4538,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4546,7 +4571,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4579,7 +4604,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4612,7 +4637,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -4645,7 +4670,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -4678,7 +4703,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -4711,7 +4736,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -4744,7 +4769,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -4777,7 +4802,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -4810,7 +4835,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -4843,7 +4868,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -4876,7 +4901,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -4909,7 +4934,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -4942,7 +4967,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -4975,7 +5000,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5008,7 +5033,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="246.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="255" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5041,7 +5066,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5074,7 +5099,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5107,7 +5132,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5140,7 +5165,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -5173,7 +5198,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -5206,7 +5231,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -5239,7 +5264,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -5272,7 +5297,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="87" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -5305,7 +5330,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -5338,7 +5363,7 @@
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -5371,7 +5396,7 @@
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -5404,7 +5429,7 @@
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -5437,7 +5462,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5470,7 +5495,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5503,7 +5528,7 @@
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -5536,7 +5561,7 @@
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -5569,7 +5594,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -5602,7 +5627,7 @@
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="174" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -5635,7 +5660,7 @@
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -5668,7 +5693,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -5701,7 +5726,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="304.5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" ht="315" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -5734,7 +5759,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -5767,7 +5792,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -5800,7 +5825,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -5833,7 +5858,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5868,7 +5893,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -5901,7 +5926,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -5936,7 +5961,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -5971,7 +5996,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -6004,7 +6029,7 @@
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -6039,7 +6064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -6072,7 +6097,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -6105,7 +6130,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -6138,7 +6163,7 @@
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -6171,7 +6196,7 @@
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -6204,7 +6229,7 @@
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -6237,7 +6262,7 @@
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -6272,7 +6297,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -6305,7 +6330,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -6338,7 +6363,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -6371,7 +6396,7 @@
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -6404,7 +6429,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -6437,7 +6462,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="87" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:11" ht="90" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -6470,7 +6495,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
@@ -6497,7 +6522,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>170</v>
       </c>
@@ -6530,7 +6555,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>170</v>
       </c>
@@ -6563,7 +6588,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>170</v>
       </c>
@@ -6596,7 +6621,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>170</v>
       </c>
@@ -6629,7 +6654,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -6662,7 +6687,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>170</v>
       </c>
@@ -6695,7 +6720,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>170</v>
       </c>
@@ -6728,7 +6753,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -6761,7 +6786,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>170</v>
       </c>
@@ -6794,7 +6819,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -6827,7 +6852,7 @@
       </c>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>170</v>
       </c>
@@ -6860,7 +6885,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>170</v>
       </c>
@@ -6893,7 +6918,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -6926,7 +6951,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -6959,7 +6984,7 @@
       </c>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>170</v>
       </c>
@@ -6992,7 +7017,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>170</v>
       </c>
@@ -7017,7 +7042,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -7042,7 +7067,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -7067,7 +7092,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -7092,7 +7117,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -7117,7 +7142,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>170</v>
       </c>
@@ -7133,7 +7158,9 @@
       <c r="E89" s="13">
         <v>44635</v>
       </c>
-      <c r="F89" s="2"/>
+      <c r="F89" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="G89" s="14">
         <v>44641</v>
       </c>
@@ -7142,7 +7169,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>170</v>
       </c>
@@ -7158,7 +7185,9 @@
       <c r="E90" s="13">
         <v>44635</v>
       </c>
-      <c r="F90" s="2"/>
+      <c r="F90" s="2" t="s">
+        <v>252</v>
+      </c>
       <c r="G90" s="14">
         <v>44641</v>
       </c>
@@ -7167,7 +7196,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>170</v>
       </c>
@@ -7192,7 +7221,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>170</v>
       </c>
@@ -7208,7 +7237,9 @@
       <c r="E92" s="13">
         <v>44635</v>
       </c>
-      <c r="F92" s="2"/>
+      <c r="F92" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="G92" s="14">
         <v>44641</v>
       </c>
@@ -7216,6 +7247,31 @@
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E93" s="13">
+        <v>44638</v>
+      </c>
+      <c r="F93" s="2"/>
+      <c r="G93" s="14">
+        <v>44642</v>
+      </c>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K92" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -7232,15 +7288,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1727200</xdr:colOff>
+                <xdr:colOff>1729740</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>50800</xdr:rowOff>
+                <xdr:rowOff>53340</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2216150</xdr:colOff>
+                <xdr:colOff>2217420</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>330200</xdr:rowOff>
+                <xdr:rowOff>327660</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7257,15 +7313,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2311400</xdr:colOff>
+                <xdr:colOff>2308860</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>222250</xdr:rowOff>
+                <xdr:rowOff>220980</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>2933700</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>539750</xdr:rowOff>
+                <xdr:rowOff>541020</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7287,20 +7343,20 @@
       <selection activeCell="A16" sqref="A16:T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="19" width="5.6328125" customWidth="1"/>
-    <col min="20" max="20" width="8.6328125" customWidth="1"/>
-    <col min="21" max="21" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="19" width="5.6640625" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>235</v>
       </c>
@@ -7332,7 +7388,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>233</v>
       </c>
@@ -7385,7 +7441,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>161</v>
       </c>
@@ -7420,7 +7476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>44575</v>
       </c>
@@ -7451,7 +7507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>44587</v>
       </c>
@@ -7482,7 +7538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>44589</v>
       </c>
@@ -7513,7 +7569,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>44615</v>
       </c>
@@ -7550,7 +7606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>44635</v>
       </c>
@@ -7579,7 +7635,7 @@
       </c>
       <c r="S11" s="29"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
         <v>169</v>
       </c>
@@ -7634,7 +7690,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>220</v>
       </c>
@@ -7676,12 +7732,12 @@
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>245</v>
       </c>
       <c r="B17" s="35" t="str">
-        <f t="shared" ref="A17:S17" si="0">B5</f>
+        <f t="shared" ref="B17:Q17" si="0">B5</f>
         <v>預計</v>
       </c>
       <c r="C17" s="35" t="str">
@@ -7754,12 +7810,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>246</v>
       </c>
       <c r="B18" s="17">
-        <f t="shared" ref="A18:S18" si="1">B6</f>
+        <f t="shared" ref="B18:S18" si="1">B6</f>
         <v>0</v>
       </c>
       <c r="C18" s="17">
@@ -7835,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="32">
         <f t="shared" ref="A19:S19" si="2">A7</f>
         <v>44575</v>
@@ -7917,7 +7973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
         <f t="shared" ref="A20:S20" si="4">A8</f>
         <v>44587</v>
@@ -7999,7 +8055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="32">
         <f t="shared" ref="A21:S21" si="5">A9</f>
         <v>44589</v>
@@ -8081,7 +8137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="32">
         <f t="shared" ref="A22:S22" si="6">A10</f>
         <v>44615</v>
@@ -8163,7 +8219,7 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="32">
         <f t="shared" ref="A23:S23" si="7">A11</f>
         <v>44635</v>
@@ -8245,7 +8301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="str">
         <f t="shared" ref="A24:S24" si="8">A12</f>
         <v>總計</v>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/22 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659FD4B7-600C-4043-94F1-21474908A04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7B7456-900E-4DCE-99ED-2F7C188A019B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="63" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="255">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1207,10 +1207,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2022/2/8、11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>程慧娟</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1220,10 +1216,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>L8950、L8350、L8351</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>銷號欄開放輸入</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1241,6 +1233,15 @@
   </si>
   <si>
     <t>新增連動保證人資料查詢雨火險資料查詢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聯徵MU1爆送：L8950、L8350、L8351</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.程式調整
+2.以代碼交易調整</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1525,7 +1526,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
@@ -1569,18 +1570,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53789</xdr:colOff>
+      <xdr:colOff>47438</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>632013</xdr:rowOff>
+      <xdr:rowOff>568512</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2300733</xdr:colOff>
+      <xdr:colOff>2535567</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1523553</xdr:rowOff>
+      <xdr:rowOff>1555749</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1603,8 +1604,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6366436" y="7631954"/>
-          <a:ext cx="2246944" cy="891540"/>
+          <a:off x="5495738" y="7566212"/>
+          <a:ext cx="2488129" cy="987237"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1613,7 +1614,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>83821</xdr:colOff>
@@ -1663,7 +1664,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
@@ -1713,7 +1714,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2304784</xdr:colOff>
@@ -1763,18 +1764,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:colOff>46990</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>480060</xdr:rowOff>
+      <xdr:rowOff>314960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3209703</xdr:colOff>
+      <xdr:colOff>3834714</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1196535</xdr:rowOff>
+      <xdr:rowOff>1174750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1803,8 +1804,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7048500" y="11148060"/>
-          <a:ext cx="3156363" cy="716475"/>
+          <a:off x="5495290" y="15231110"/>
+          <a:ext cx="3787724" cy="859790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1813,18 +1814,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>97140</xdr:colOff>
+      <xdr:colOff>33640</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1760221</xdr:rowOff>
+      <xdr:rowOff>1614171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1936378</xdr:colOff>
+      <xdr:colOff>2117834</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>2627670</xdr:rowOff>
+      <xdr:rowOff>2597150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1853,8 +1854,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7098575" y="12419256"/>
-          <a:ext cx="1839238" cy="867449"/>
+          <a:off x="5481940" y="16530321"/>
+          <a:ext cx="2084194" cy="982979"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1863,18 +1864,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2105188</xdr:colOff>
+      <xdr:colOff>2155988</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1731659</xdr:rowOff>
+      <xdr:rowOff>1585608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>4455459</xdr:colOff>
+      <xdr:colOff>4701437</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>2671501</xdr:rowOff>
+      <xdr:rowOff>2603499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1903,8 +1904,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9106623" y="12390694"/>
-          <a:ext cx="2350271" cy="939842"/>
+          <a:off x="7604288" y="16501758"/>
+          <a:ext cx="2545449" cy="1017891"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1913,7 +1914,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1008829</xdr:colOff>
@@ -1956,7 +1957,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>926353</xdr:colOff>
@@ -1999,7 +2000,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>22861</xdr:colOff>
@@ -2043,7 +2044,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
@@ -2087,7 +2088,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
@@ -2131,7 +2132,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2317974</xdr:colOff>
@@ -2175,16 +2176,16 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1100420</xdr:colOff>
+      <xdr:colOff>1119470</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>173196</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>4452471</xdr:colOff>
+      <xdr:colOff>4471521</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>679023</xdr:rowOff>
     </xdr:to>
@@ -2209,7 +2210,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7413067" y="39632843"/>
+          <a:off x="6567770" y="40362346"/>
           <a:ext cx="3352051" cy="505827"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2219,7 +2220,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
@@ -2263,7 +2264,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>32078</xdr:colOff>
@@ -2307,7 +2308,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>55360</xdr:colOff>
@@ -2351,18 +2352,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>32158</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>1924050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3947046</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>533133</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>2825483</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2385,7 +2386,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5480458" y="368300"/>
+          <a:off x="5480458" y="46901100"/>
           <a:ext cx="3914888" cy="901433"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2395,18 +2396,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>2750820</xdr:rowOff>
+      <xdr:rowOff>2731770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3832859</xdr:colOff>
+      <xdr:colOff>3813809</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>3865880</xdr:rowOff>
+      <xdr:rowOff>3846830</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2429,8 +2430,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5585460" y="50962560"/>
-          <a:ext cx="3756659" cy="1242060"/>
+          <a:off x="5505450" y="47708820"/>
+          <a:ext cx="3756659" cy="1115060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2441,18 +2442,18 @@
   </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1729740</xdr:colOff>
+          <xdr:colOff>1727200</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>50800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2217420</xdr:colOff>
+          <xdr:colOff>2216150</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>327660</xdr:rowOff>
+          <xdr:rowOff>330200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2496,18 +2497,18 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2308860</xdr:colOff>
+          <xdr:colOff>2311400</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>220980</xdr:rowOff>
+          <xdr:rowOff>222250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>2933700</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>541020</xdr:rowOff>
+          <xdr:rowOff>539750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2553,7 +2554,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44635.785155555554" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="92" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44642.540675462966" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="93" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K1048576" sheet="User審查意見彙整"/>
   </cacheSource>
@@ -2571,13 +2572,14 @@
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
     <cacheField name="意見收到日" numFmtId="14">
-      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2022-01-14T00:00:00" maxDate="2022-03-16T00:00:00" count="7">
+      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2022-01-14T00:00:00" maxDate="2022-03-19T00:00:00" count="8">
         <d v="2022-01-14T00:00:00"/>
         <d v="2022-01-26T00:00:00"/>
         <d v="2022-01-28T00:00:00"/>
         <s v="2022/2/8、2022/2/11"/>
         <d v="2022-02-23T00:00:00"/>
         <d v="2022-03-15T00:00:00"/>
+        <d v="2022-03-18T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -2619,7 +2621,7 @@
       </fieldGroup>
     </cacheField>
     <cacheField name="意見回覆日" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-16T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-23T00:00:00"/>
     </cacheField>
     <cacheField name="回覆狀態" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -2640,7 +2642,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="92">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="93">
   <r>
     <s v="邵淑微"/>
     <n v="1"/>
@@ -3507,8 +3509,8 @@
     <x v="4"/>
     <s v="戶號改為區間查詢"/>
     <x v="5"/>
-    <m/>
-    <m/>
+    <d v="2022-03-22T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3726,7 +3728,7 @@
     <s v="L2631清償作業"/>
     <s v="關於保證及火險查詢：無此設計"/>
     <x v="5"/>
-    <m/>
+    <s v="新增連動保證人資料查詢雨火險資料查詢"/>
     <x v="10"/>
     <m/>
     <m/>
@@ -3752,10 +3754,10 @@
     <s v="L2631清償作業"/>
     <s v="領取日期：此欄位不用"/>
     <x v="5"/>
-    <m/>
+    <s v="已刪除此欄位"/>
     <x v="10"/>
-    <m/>
-    <m/>
+    <d v="2022-03-22T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3778,10 +3780,10 @@
     <s v="L2631清償作業"/>
     <s v="是否有判斷，同押品是否同時要結清或是餘額為0，才可領取清償證明。"/>
     <x v="5"/>
-    <m/>
+    <s v="有判斷此額度已全部結清才可領取清償證明"/>
     <x v="11"/>
-    <m/>
-    <m/>
+    <d v="2022-03-22T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3791,10 +3793,10 @@
     <s v="L2631清償作業"/>
     <s v="關於申請日期，應為系統之日曆日，非會計日"/>
     <x v="5"/>
-    <m/>
+    <s v="已修正"/>
     <x v="11"/>
-    <m/>
-    <m/>
+    <d v="2022-03-22T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3817,19 +3819,32 @@
     <s v="L2632清償作業維護"/>
     <s v="已結清時，銷號欄要可輸入"/>
     <x v="5"/>
-    <m/>
+    <s v="銷號欄開放輸入"/>
     <x v="11"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <d v="2022-03-22T00:00:00"/>
+    <s v="已完成"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="程慧娟"/>
+    <n v="1"/>
+    <s v="L8950、L8350、L8351"/>
+    <s v="1.授權辦理事項：三個選項應為■查詢■覆核■其他，請將系統第一個選項審查更改為查詢。_x000a_2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。"/>
     <x v="6"/>
+    <m/>
+    <x v="5"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="7"/>
     <m/>
     <x v="12"/>
     <m/>
@@ -3841,22 +3856,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:S12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="63" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:S13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="8">
+      <items count="9">
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="4"/>
         <item x="5"/>
-        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3886,7 +3902,7 @@
   <rowFields count="1">
     <field x="4"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="8">
     <i>
       <x/>
     </i>
@@ -3904,6 +3920,9 @@
     </i>
     <i>
       <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -4258,29 +4277,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
+      <selection pane="bottomLeft" activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="44.6328125" style="16" customWidth="1"/>
     <col min="5" max="5" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="67.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>162</v>
       </c>
@@ -4315,7 +4334,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4348,7 +4367,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -4381,7 +4400,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4414,7 +4433,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -4447,7 +4466,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4480,7 +4499,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4513,7 +4532,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4546,7 +4565,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4579,7 +4598,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4612,7 +4631,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4645,7 +4664,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -4678,7 +4697,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -4711,7 +4730,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -4744,7 +4763,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -4777,7 +4796,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -4810,7 +4829,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -4843,7 +4862,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -4876,7 +4895,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -4909,7 +4928,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -4942,7 +4961,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -4975,7 +4994,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5008,7 +5027,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="409.5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5041,7 +5060,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="255" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="246.5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5074,7 +5093,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5107,7 +5126,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5140,7 +5159,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5173,7 +5192,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -5206,7 +5225,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -5239,7 +5258,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -5272,7 +5291,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -5305,7 +5324,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="87" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -5338,7 +5357,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -5371,7 +5390,7 @@
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -5404,7 +5423,7 @@
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -5437,7 +5456,7 @@
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -5470,7 +5489,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5503,7 +5522,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5536,7 +5555,7 @@
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -5569,7 +5588,7 @@
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -5602,7 +5621,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -5635,7 +5654,7 @@
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="174" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -5668,7 +5687,7 @@
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -5701,7 +5720,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -5734,7 +5753,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="315" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="304.5" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -5767,7 +5786,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -5800,7 +5819,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -5833,7 +5852,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -5866,7 +5885,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5901,7 +5920,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -5934,7 +5953,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -5969,7 +5988,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -6004,7 +6023,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -6037,7 +6056,7 @@
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -6072,7 +6091,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -6105,7 +6124,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -6138,7 +6157,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -6171,7 +6190,7 @@
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -6204,7 +6223,7 @@
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -6237,7 +6256,7 @@
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -6270,7 +6289,7 @@
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -6305,7 +6324,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -6338,7 +6357,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -6371,7 +6390,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -6404,7 +6423,7 @@
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -6437,7 +6456,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -6470,7 +6489,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="87" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -6503,7 +6522,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
@@ -6525,12 +6544,16 @@
       <c r="G68" s="14">
         <v>44642</v>
       </c>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
+      <c r="H68" s="11">
+        <v>44642</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>170</v>
       </c>
@@ -6563,7 +6586,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>170</v>
       </c>
@@ -6596,7 +6619,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>170</v>
       </c>
@@ -6629,7 +6652,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>170</v>
       </c>
@@ -6662,7 +6685,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -6695,7 +6718,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>170</v>
       </c>
@@ -6728,7 +6751,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>170</v>
       </c>
@@ -6761,7 +6784,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -6794,7 +6817,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>170</v>
       </c>
@@ -6827,7 +6850,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -6860,7 +6883,7 @@
       </c>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>170</v>
       </c>
@@ -6893,7 +6916,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>170</v>
       </c>
@@ -6926,7 +6949,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -6959,7 +6982,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -6992,7 +7015,7 @@
       </c>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>170</v>
       </c>
@@ -7025,7 +7048,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>170</v>
       </c>
@@ -7050,7 +7073,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -7067,7 +7090,7 @@
         <v>44635</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G85" s="14">
         <v>44643</v>
@@ -7077,7 +7100,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -7102,7 +7125,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -7119,17 +7142,21 @@
         <v>44635</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G87" s="14">
         <v>44643</v>
       </c>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
+      <c r="H87" s="11">
+        <v>44642</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -7154,7 +7181,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>170</v>
       </c>
@@ -7171,17 +7198,21 @@
         <v>44635</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G89" s="14">
         <v>44641</v>
       </c>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
+      <c r="H89" s="11">
+        <v>44642</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>170</v>
       </c>
@@ -7198,17 +7229,21 @@
         <v>44635</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G90" s="14">
         <v>44641</v>
       </c>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
+      <c r="H90" s="11">
+        <v>44642</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>170</v>
       </c>
@@ -7233,7 +7268,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>170</v>
       </c>
@@ -7250,38 +7285,48 @@
         <v>44635</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G92" s="14">
         <v>44641</v>
       </c>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
+      <c r="H92" s="11">
+        <v>44642</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B93" s="2">
         <v>1</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E93" s="13">
         <v>44638</v>
       </c>
-      <c r="F93" s="2"/>
+      <c r="F93" s="6" t="s">
+        <v>254</v>
+      </c>
       <c r="G93" s="14">
         <v>44642</v>
       </c>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
+      <c r="H93" s="11">
+        <v>44641</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
@@ -7297,18 +7342,18 @@
       <mc:Choice Requires="x14">
         <oleObject progId="封裝程式殼層物件" shapeId="1025" r:id="rId4">
           <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1">
+            <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1729740</xdr:colOff>
+                <xdr:colOff>1727200</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>53340</xdr:rowOff>
+                <xdr:rowOff>50800</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2217420</xdr:colOff>
+                <xdr:colOff>2216150</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>327660</xdr:rowOff>
+                <xdr:rowOff>330200</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7322,18 +7367,18 @@
       <mc:Choice Requires="x14">
         <oleObject progId="封裝程式殼層物件" shapeId="1026" r:id="rId6">
           <objectPr defaultSize="0" autoPict="0" r:id="rId7">
-            <anchor moveWithCells="1">
+            <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2308860</xdr:colOff>
+                <xdr:colOff>2311400</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>220980</xdr:rowOff>
+                <xdr:rowOff>222250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>2933700</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>541020</xdr:rowOff>
+                <xdr:rowOff>539750</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7349,26 +7394,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E69748B-F013-4C3D-B545-0E0A517A1BB7}">
-  <dimension ref="A3:T24"/>
+  <dimension ref="A3:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:T24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="19" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="5.6328125" customWidth="1"/>
+    <col min="21" max="21" width="28.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>235</v>
       </c>
@@ -7400,7 +7444,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A5" s="27" t="s">
         <v>233</v>
       </c>
@@ -7453,7 +7497,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A6" s="28" t="s">
         <v>161</v>
       </c>
@@ -7488,7 +7532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A7" s="30">
         <v>44575</v>
       </c>
@@ -7519,7 +7563,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A8" s="30">
         <v>44587</v>
       </c>
@@ -7550,7 +7594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" s="30">
         <v>44589</v>
       </c>
@@ -7581,7 +7625,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A10" s="30">
         <v>44615</v>
       </c>
@@ -7608,17 +7652,19 @@
       <c r="N10" s="29">
         <v>1</v>
       </c>
-      <c r="O10" s="29"/>
+      <c r="O10" s="29">
+        <v>1</v>
+      </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
       <c r="R10" s="29">
         <v>16</v>
       </c>
       <c r="S10" s="29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" s="30">
         <v>44635</v>
       </c>
@@ -7637,7 +7683,9 @@
       <c r="N11" s="29">
         <v>7</v>
       </c>
-      <c r="O11" s="29"/>
+      <c r="O11" s="29">
+        <v>4</v>
+      </c>
       <c r="P11" s="29">
         <v>2</v>
       </c>
@@ -7645,64 +7693,95 @@
       <c r="R11" s="29">
         <v>9</v>
       </c>
-      <c r="S11" s="29"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12" s="29">
-        <v>21</v>
-      </c>
-      <c r="C12" s="29">
-        <v>21</v>
-      </c>
-      <c r="D12" s="29">
-        <v>22</v>
-      </c>
-      <c r="E12" s="29">
-        <v>22</v>
-      </c>
-      <c r="F12" s="29">
-        <v>22</v>
-      </c>
-      <c r="G12" s="29">
-        <v>22</v>
-      </c>
-      <c r="H12" s="29">
+      <c r="S11" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A12" s="30">
+        <v>44638</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29">
         <v>1</v>
       </c>
-      <c r="I12" s="29">
-        <v>1</v>
-      </c>
-      <c r="J12" s="29">
-        <v>3</v>
-      </c>
-      <c r="K12" s="29">
-        <v>3</v>
-      </c>
-      <c r="L12" s="29">
-        <v>12</v>
-      </c>
-      <c r="M12" s="29">
-        <v>12</v>
-      </c>
-      <c r="N12" s="29">
-        <v>8</v>
-      </c>
       <c r="O12" s="29"/>
-      <c r="P12" s="29">
-        <v>2</v>
-      </c>
+      <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="29">
-        <v>91</v>
-      </c>
-      <c r="S12" s="29">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="S12" s="29"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A13" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="29">
+        <v>21</v>
+      </c>
+      <c r="C13" s="29">
+        <v>21</v>
+      </c>
+      <c r="D13" s="29">
+        <v>22</v>
+      </c>
+      <c r="E13" s="29">
+        <v>22</v>
+      </c>
+      <c r="F13" s="29">
+        <v>22</v>
+      </c>
+      <c r="G13" s="29">
+        <v>22</v>
+      </c>
+      <c r="H13" s="29">
+        <v>1</v>
+      </c>
+      <c r="I13" s="29">
+        <v>1</v>
+      </c>
+      <c r="J13" s="29">
+        <v>3</v>
+      </c>
+      <c r="K13" s="29">
+        <v>3</v>
+      </c>
+      <c r="L13" s="29">
+        <v>12</v>
+      </c>
+      <c r="M13" s="29">
+        <v>12</v>
+      </c>
+      <c r="N13" s="29">
+        <v>9</v>
+      </c>
+      <c r="O13" s="29">
+        <v>5</v>
+      </c>
+      <c r="P13" s="29">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29">
+        <v>92</v>
+      </c>
+      <c r="S13" s="29">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="34" t="s">
         <v>220</v>
       </c>
@@ -7744,7 +7823,7 @@
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A17" s="35" t="s">
         <v>245</v>
       </c>
@@ -7822,12 +7901,13 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>246</v>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A18" s="17" t="str">
+        <f t="shared" ref="A18:S18" si="1">A6</f>
+        <v>2022/2/8、2022/2/11</v>
       </c>
       <c r="B18" s="17">
-        <f t="shared" ref="B18:S18" si="1">B6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C18" s="17">
@@ -7903,7 +7983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A19" s="32">
         <f t="shared" ref="A19:S19" si="2">A7</f>
         <v>44575</v>
@@ -7981,11 +8061,11 @@
         <v>21</v>
       </c>
       <c r="T19" s="25">
-        <f t="shared" ref="T19:T24" si="3">S19/R19</f>
+        <f t="shared" ref="T19:T25" si="3">S19/R19</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A20" s="32">
         <f t="shared" ref="A20:S20" si="4">A8</f>
         <v>44587</v>
@@ -8067,7 +8147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A21" s="32">
         <f t="shared" ref="A21:S21" si="5">A9</f>
         <v>44589</v>
@@ -8149,7 +8229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A22" s="32">
         <f t="shared" ref="A22:S22" si="6">A10</f>
         <v>44615</v>
@@ -8208,7 +8288,7 @@
       </c>
       <c r="O22" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="17">
         <f t="shared" si="6"/>
@@ -8224,14 +8304,14 @@
       </c>
       <c r="S22" s="18">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="T22" s="25">
         <f t="shared" si="3"/>
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A23" s="32">
         <f t="shared" ref="A23:S23" si="7">A11</f>
         <v>44635</v>
@@ -8290,7 +8370,7 @@
       </c>
       <c r="O23" s="17">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P23" s="17">
         <f t="shared" si="7"/>
@@ -8306,93 +8386,172 @@
       </c>
       <c r="S23" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T23" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="str">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A24" s="32">
         <f t="shared" ref="A24:S24" si="8">A12</f>
-        <v>總計</v>
-      </c>
-      <c r="B24" s="35">
+        <v>44638</v>
+      </c>
+      <c r="B24" s="17">
         <f t="shared" si="8"/>
-        <v>21</v>
-      </c>
-      <c r="C24" s="35">
+        <v>0</v>
+      </c>
+      <c r="C24" s="17">
         <f t="shared" si="8"/>
-        <v>21</v>
-      </c>
-      <c r="D24" s="35">
+        <v>0</v>
+      </c>
+      <c r="D24" s="17">
         <f t="shared" si="8"/>
-        <v>22</v>
-      </c>
-      <c r="E24" s="35">
+        <v>0</v>
+      </c>
+      <c r="E24" s="17">
         <f t="shared" si="8"/>
-        <v>22</v>
-      </c>
-      <c r="F24" s="35">
+        <v>0</v>
+      </c>
+      <c r="F24" s="17">
         <f t="shared" si="8"/>
-        <v>22</v>
-      </c>
-      <c r="G24" s="35">
+        <v>0</v>
+      </c>
+      <c r="G24" s="17">
         <f t="shared" si="8"/>
-        <v>22</v>
-      </c>
-      <c r="H24" s="35">
+        <v>0</v>
+      </c>
+      <c r="H24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="17">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="I24" s="35">
+      <c r="O24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="18">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="J24" s="35">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="K24" s="35">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="L24" s="35">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="M24" s="35">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="N24" s="35">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="O24" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="35">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="Q24" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="18">
-        <f t="shared" si="8"/>
-        <v>91</v>
-      </c>
       <c r="S24" s="18">
         <f t="shared" si="8"/>
-        <v>81</v>
-      </c>
-      <c r="T24" s="25">
+        <v>0</v>
+      </c>
+      <c r="T24" s="25"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A25" s="35" t="str">
+        <f t="shared" ref="A25:S25" si="9">A13</f>
+        <v>總計</v>
+      </c>
+      <c r="B25" s="35">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="C25" s="35">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="35">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="E25" s="35">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="F25" s="35">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="G25" s="35">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="H25" s="35">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="35">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="35">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="K25" s="35">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="L25" s="35">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="M25" s="35">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="N25" s="35">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="O25" s="35">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="P25" s="35">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="Q25" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="18">
+        <f t="shared" si="9"/>
+        <v>92</v>
+      </c>
+      <c r="S25" s="18">
+        <f t="shared" si="9"/>
+        <v>86</v>
+      </c>
+      <c r="T25" s="25">
         <f t="shared" si="3"/>
-        <v>0.89010989010989006</v>
+        <v>0.93478260869565222</v>
       </c>
     </row>
   </sheetData>
@@ -8402,6 +8561,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -8515,33 +8689,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8562,9 +8713,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/23 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0119F124-E258-4D08-98C2-6AE2F0F02A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACB0360-A9C6-47CD-B231-D1779509E424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="257">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1220,10 +1220,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>有判斷此額度已全部結清才可領取清償證明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>已修正</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1242,6 +1238,18 @@
   </si>
   <si>
     <t>新增連動[L2902 保證人保證資料查詢]與[L4960 火險保費資料查詢(By客戶)]</t>
+  </si>
+  <si>
+    <t>入帳日與金額可修改,金額依入帳日預設可修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>問佩瑜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判斷擔保品需全部結案才可領取清償證明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1332,7 +1340,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1360,6 +1368,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1396,7 +1410,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1504,6 +1518,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4277,9 +4303,9 @@
   <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -7057,13 +7083,13 @@
       <c r="C84" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="E84" s="13">
+      <c r="E84" s="37">
         <v>44635</v>
       </c>
-      <c r="F84" s="2"/>
+      <c r="F84" s="38"/>
       <c r="G84" s="14">
         <v>44649</v>
       </c>
@@ -7089,7 +7115,7 @@
         <v>44635</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G85" s="14">
         <v>44643</v>
@@ -7113,13 +7139,13 @@
       <c r="C86" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="E86" s="13">
+      <c r="E86" s="37">
         <v>44635</v>
       </c>
-      <c r="F86" s="2"/>
+      <c r="F86" s="38"/>
       <c r="G86" s="14">
         <v>44641</v>
       </c>
@@ -7145,7 +7171,7 @@
         <v>44635</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G87" s="14">
         <v>44643</v>
@@ -7169,13 +7195,15 @@
       <c r="C88" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="E88" s="13">
+      <c r="E88" s="37">
         <v>44635</v>
       </c>
-      <c r="F88" s="2"/>
+      <c r="F88" s="38" t="s">
+        <v>255</v>
+      </c>
       <c r="G88" s="14">
         <v>44649</v>
       </c>
@@ -7194,14 +7222,14 @@
       <c r="C89" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="E89" s="13">
+      <c r="E89" s="37">
         <v>44635</v>
       </c>
-      <c r="F89" s="2" t="s">
-        <v>249</v>
+      <c r="F89" s="38" t="s">
+        <v>256</v>
       </c>
       <c r="G89" s="14">
         <v>44641</v>
@@ -7232,7 +7260,7 @@
         <v>44635</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G90" s="14">
         <v>44641</v>
@@ -7256,13 +7284,15 @@
       <c r="C91" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D91" s="26" t="s">
+      <c r="D91" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="E91" s="13">
+      <c r="E91" s="37">
         <v>44635</v>
       </c>
-      <c r="F91" s="2"/>
+      <c r="F91" s="38" t="s">
+        <v>254</v>
+      </c>
       <c r="G91" s="14">
         <v>44641</v>
       </c>
@@ -7310,7 +7340,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>247</v>
@@ -7319,7 +7349,7 @@
         <v>44638</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G93" s="14">
         <v>44642</v>
@@ -8564,21 +8594,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -8692,17 +8707,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8716,17 +8747,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/24 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACB0360-A9C6-47CD-B231-D1779509E424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2223D4C8-3FDD-4885-BCAC-03E626491A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
@@ -4305,7 +4305,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
+      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/03/25 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2223D4C8-3FDD-4885-BCAC-03E626491A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AC7606-B359-487C-85DA-920F53897978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="3570" yWindow="190" windowWidth="13720" windowHeight="9780" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
     <sheet name="工作表2" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">User審查意見彙整!$A$1:$K$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">User審查意見彙整!$A$1:$K$93</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1232,23 +1232,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.程式調整
+    <t>新增連動[L2902 保證人保證資料查詢]與[L4960 火險保費資料查詢(By客戶)]</t>
+  </si>
+  <si>
+    <t>入帳日與金額可修改,金額依入帳日預設可修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>問佩瑜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判斷擔保品需全部結案才可領取清償證明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.URS、程式調整
 2.以代碼交易調整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增連動[L2902 保證人保證資料查詢]與[L4960 火險保費資料查詢(By客戶)]</t>
-  </si>
-  <si>
-    <t>入帳日與金額可修改,金額依入帳日預設可修改</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>問佩瑜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>判斷擔保品需全部結案才可領取清償證明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1259,7 +1259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1339,6 +1339,13 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1410,7 +1417,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1530,6 +1537,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2470,15 +2480,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1729740</xdr:colOff>
+          <xdr:colOff>1727200</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>50800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2217420</xdr:colOff>
+          <xdr:colOff>2216150</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>327660</xdr:rowOff>
+          <xdr:rowOff>330200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2525,15 +2535,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2308860</xdr:colOff>
+          <xdr:colOff>2311400</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>220980</xdr:rowOff>
+          <xdr:rowOff>222250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>2933700</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>541020</xdr:rowOff>
+          <xdr:rowOff>539750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2579,7 +2589,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44642.540675462966" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="93" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44645.46858645833" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="93" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K1048576" sheet="User審查意見彙整"/>
   </cacheSource>
@@ -3753,10 +3763,10 @@
     <s v="L2631清償作業"/>
     <s v="關於保證及火險查詢：無此設計"/>
     <x v="5"/>
-    <s v="新增連動保證人資料查詢雨火險資料查詢"/>
+    <s v="新增連動[L2902 保證人保證資料查詢]與[L4960 火險保費資料查詢(By客戶)]"/>
     <x v="10"/>
-    <m/>
-    <m/>
+    <d v="2022-03-22T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3767,7 +3777,7 @@
     <s v="登錄後列印文件：如附件"/>
     <x v="5"/>
     <m/>
-    <x v="11"/>
+    <x v="9"/>
     <m/>
     <m/>
     <m/>
@@ -3792,7 +3802,7 @@
     <s v="L2631清償作業"/>
     <s v="當初有提到可以多額度選取，請問如果要選擇1跟4額度時，要如何處理?"/>
     <x v="5"/>
-    <m/>
+    <s v="問佩瑜"/>
     <x v="9"/>
     <m/>
     <m/>
@@ -3805,7 +3815,7 @@
     <s v="L2631清償作業"/>
     <s v="是否有判斷，同押品是否同時要結清或是餘額為0，才可領取清償證明。"/>
     <x v="5"/>
-    <s v="有判斷此額度已全部結清才可領取清償證明"/>
+    <s v="判斷擔保品需全部結案才可領取清償證明"/>
     <x v="11"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
@@ -3831,8 +3841,8 @@
     <s v="L2632清償作業維護"/>
     <s v="未結清時，修改金額，而非修改入帳日"/>
     <x v="5"/>
-    <m/>
-    <x v="11"/>
+    <s v="入帳日與金額可修改,金額依入帳日預設可修改"/>
+    <x v="9"/>
     <m/>
     <m/>
     <m/>
@@ -3854,13 +3864,13 @@
   <r>
     <s v="程慧娟"/>
     <n v="1"/>
-    <s v="L8950、L8350、L8351"/>
+    <s v="聯徵MU1爆送：L8950、L8350、L8351"/>
     <s v="1.授權辦理事項：三個選項應為■查詢■覆核■其他，請將系統第一個選項審查更改為查詢。_x000a_2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。"/>
     <x v="6"/>
-    <m/>
+    <s v="1.程式調整_x000a_2.以代碼交易調整"/>
     <x v="5"/>
-    <m/>
-    <m/>
+    <d v="2022-03-21T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3881,7 +3891,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:S13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -4302,29 +4312,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
+      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="44.6328125" style="16" customWidth="1"/>
     <col min="5" max="5" width="13" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>162</v>
       </c>
@@ -4359,7 +4369,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4392,7 +4402,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -4425,7 +4435,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4458,7 +4468,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -4491,7 +4501,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4524,7 +4534,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4557,7 +4567,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4590,7 +4600,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4623,7 +4633,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4656,7 +4666,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4689,7 +4699,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -4722,7 +4732,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -4755,7 +4765,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -4788,7 +4798,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -4821,7 +4831,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -4854,7 +4864,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -4887,7 +4897,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -4920,7 +4930,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -4953,7 +4963,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -4986,7 +4996,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -5019,7 +5029,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5052,7 +5062,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="409.5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5085,7 +5095,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="255" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="275.5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5118,7 +5128,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5151,7 +5161,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5184,7 +5194,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5217,7 +5227,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -5250,7 +5260,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -5283,7 +5293,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -5316,7 +5326,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -5349,7 +5359,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="87" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -5382,7 +5392,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -5415,7 +5425,7 @@
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -5448,7 +5458,7 @@
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -5481,7 +5491,7 @@
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -5514,7 +5524,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5547,7 +5557,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5580,7 +5590,7 @@
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -5613,7 +5623,7 @@
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -5646,7 +5656,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -5679,7 +5689,7 @@
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="174" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -5712,7 +5722,7 @@
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -5745,7 +5755,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -5778,7 +5788,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="315" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="333.5" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -5811,7 +5821,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -5844,7 +5854,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -5877,7 +5887,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -5910,7 +5920,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5945,7 +5955,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -5978,7 +5988,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -6013,7 +6023,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -6048,7 +6058,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -6081,7 +6091,7 @@
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -6116,7 +6126,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -6149,7 +6159,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -6182,7 +6192,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -6215,7 +6225,7 @@
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -6248,7 +6258,7 @@
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -6281,7 +6291,7 @@
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -6314,7 +6324,7 @@
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -6349,7 +6359,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -6382,7 +6392,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -6415,7 +6425,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -6448,7 +6458,7 @@
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -6481,7 +6491,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -6514,7 +6524,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -6547,7 +6557,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
@@ -6578,7 +6588,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>170</v>
       </c>
@@ -6611,7 +6621,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>170</v>
       </c>
@@ -6644,7 +6654,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>170</v>
       </c>
@@ -6677,7 +6687,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>170</v>
       </c>
@@ -6710,7 +6720,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -6743,7 +6753,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>170</v>
       </c>
@@ -6776,7 +6786,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>170</v>
       </c>
@@ -6809,7 +6819,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -6842,7 +6852,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>170</v>
       </c>
@@ -6875,7 +6885,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -6908,7 +6918,7 @@
       </c>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>170</v>
       </c>
@@ -6941,7 +6951,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>170</v>
       </c>
@@ -6974,7 +6984,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -7007,7 +7017,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -7040,7 +7050,7 @@
       </c>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>170</v>
       </c>
@@ -7073,7 +7083,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>170</v>
       </c>
@@ -7098,7 +7108,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -7115,7 +7125,7 @@
         <v>44635</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G85" s="14">
         <v>44643</v>
@@ -7129,7 +7139,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -7147,14 +7157,14 @@
       </c>
       <c r="F86" s="38"/>
       <c r="G86" s="14">
-        <v>44641</v>
+        <v>44649</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -7185,7 +7195,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -7202,7 +7212,7 @@
         <v>44635</v>
       </c>
       <c r="F88" s="38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G88" s="14">
         <v>44649</v>
@@ -7212,7 +7222,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>170</v>
       </c>
@@ -7229,7 +7239,7 @@
         <v>44635</v>
       </c>
       <c r="F89" s="38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G89" s="14">
         <v>44641</v>
@@ -7243,7 +7253,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>170</v>
       </c>
@@ -7274,7 +7284,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>170</v>
       </c>
@@ -7291,17 +7301,17 @@
         <v>44635</v>
       </c>
       <c r="F91" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G91" s="14">
-        <v>44641</v>
+        <v>44649</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>170</v>
       </c>
@@ -7332,7 +7342,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>246</v>
       </c>
@@ -7349,7 +7359,7 @@
         <v>44638</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="G93" s="14">
         <v>44642</v>
@@ -7364,7 +7374,7 @@
       <c r="K93" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K92" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K93" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7378,15 +7388,15 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1729740</xdr:colOff>
+                <xdr:colOff>1727200</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>53340</xdr:rowOff>
+                <xdr:rowOff>50800</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2217420</xdr:colOff>
+                <xdr:colOff>2216150</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>327660</xdr:rowOff>
+                <xdr:rowOff>330200</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7403,15 +7413,15 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2308860</xdr:colOff>
+                <xdr:colOff>2311400</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>220980</xdr:rowOff>
+                <xdr:rowOff>222250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>2933700</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>541020</xdr:rowOff>
+                <xdr:rowOff>539750</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7429,23 +7439,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E69748B-F013-4C3D-B545-0E0A517A1BB7}">
   <dimension ref="A3:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="20" width="5.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="5.6328125" customWidth="1"/>
+    <col min="21" max="21" width="28.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>235</v>
       </c>
@@ -7477,7 +7487,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A5" s="27" t="s">
         <v>233</v>
       </c>
@@ -7530,7 +7540,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A6" s="28" t="s">
         <v>161</v>
       </c>
@@ -7565,7 +7575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A7" s="30">
         <v>44575</v>
       </c>
@@ -7596,7 +7606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A8" s="30">
         <v>44587</v>
       </c>
@@ -7627,7 +7637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" s="30">
         <v>44589</v>
       </c>
@@ -7658,7 +7668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A10" s="30">
         <v>44615</v>
       </c>
@@ -7697,7 +7707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A11" s="30">
         <v>44635</v>
       </c>
@@ -7714,23 +7724,23 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
       <c r="N11" s="29">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O11" s="29">
+        <v>5</v>
+      </c>
+      <c r="P11" s="29">
         <v>4</v>
-      </c>
-      <c r="P11" s="29">
-        <v>2</v>
       </c>
       <c r="Q11" s="29"/>
       <c r="R11" s="29">
         <v>9</v>
       </c>
       <c r="S11" s="29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A12" s="30">
         <v>44638</v>
       </c>
@@ -7749,15 +7759,19 @@
       <c r="N12" s="29">
         <v>1</v>
       </c>
-      <c r="O12" s="29"/>
+      <c r="O12" s="29">
+        <v>1</v>
+      </c>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="29">
         <v>1</v>
       </c>
-      <c r="S12" s="29"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S12" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A13" s="28" t="s">
         <v>169</v>
       </c>
@@ -7798,23 +7812,23 @@
         <v>12</v>
       </c>
       <c r="N13" s="29">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O13" s="29">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P13" s="29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="29"/>
       <c r="R13" s="29">
         <v>92</v>
       </c>
       <c r="S13" s="29">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="34" t="s">
         <v>220</v>
       </c>
@@ -7856,7 +7870,7 @@
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A17" s="35" t="s">
         <v>245</v>
       </c>
@@ -7934,8 +7948,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="str">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A18" s="40" t="str">
         <f t="shared" ref="A18:S18" si="1">A6</f>
         <v>2022/2/8、2022/2/11</v>
       </c>
@@ -8016,7 +8030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A19" s="32">
         <f t="shared" ref="A19:S19" si="2">A7</f>
         <v>44575</v>
@@ -8098,7 +8112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A20" s="32">
         <f t="shared" ref="A20:S20" si="4">A8</f>
         <v>44587</v>
@@ -8180,7 +8194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A21" s="32">
         <f t="shared" ref="A21:S21" si="5">A9</f>
         <v>44589</v>
@@ -8262,7 +8276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A22" s="32">
         <f t="shared" ref="A22:S22" si="6">A10</f>
         <v>44615</v>
@@ -8344,7 +8358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A23" s="32">
         <f t="shared" ref="A23:S23" si="7">A11</f>
         <v>44635</v>
@@ -8399,15 +8413,15 @@
       </c>
       <c r="N23" s="17">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O23" s="17">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P23" s="17">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q23" s="17">
         <f t="shared" si="7"/>
@@ -8419,14 +8433,14 @@
       </c>
       <c r="S23" s="18">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T23" s="25">
         <f t="shared" si="3"/>
-        <v>0.44444444444444442</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A24" s="32">
         <f t="shared" ref="A24:S24" si="8">A12</f>
         <v>44638</v>
@@ -8485,7 +8499,7 @@
       </c>
       <c r="O24" s="17">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="17">
         <f t="shared" si="8"/>
@@ -8501,11 +8515,11 @@
       </c>
       <c r="S24" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="25"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A25" s="35" t="str">
         <f t="shared" ref="A25:S25" si="9">A13</f>
         <v>總計</v>
@@ -8560,15 +8574,15 @@
       </c>
       <c r="N25" s="35">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O25" s="35">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P25" s="35">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q25" s="35">
         <f t="shared" si="9"/>
@@ -8580,16 +8594,17 @@
       </c>
       <c r="S25" s="18">
         <f t="shared" si="9"/>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T25" s="25">
         <f t="shared" si="3"/>
-        <v>0.93478260869565222</v>
+        <v>0.95652173913043481</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8708,18 +8723,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8739,14 +8754,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8759,4 +8766,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/28 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AC7606-B359-487C-85DA-920F53897978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB52625A-28F9-4E36-A48D-547D31CA67BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="190" windowWidth="13720" windowHeight="9780" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="258">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1249,6 +1249,10 @@
   <si>
     <t>1.URS、程式調整
 2.以代碼交易調整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加按鈕連動相關交易</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2480,15 +2484,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1727200</xdr:colOff>
+          <xdr:colOff>1729740</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>50800</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2216150</xdr:colOff>
+          <xdr:colOff>2217420</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>330200</xdr:rowOff>
+          <xdr:rowOff>327660</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2535,15 +2539,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2311400</xdr:colOff>
+          <xdr:colOff>2308860</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>222250</xdr:rowOff>
+          <xdr:rowOff>220980</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>2933700</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>539750</xdr:rowOff>
+          <xdr:rowOff>541020</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3891,7 +3895,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:S13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -4312,29 +4316,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6328125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="13" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>162</v>
       </c>
@@ -4369,7 +4373,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4402,7 +4406,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -4435,7 +4439,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4468,7 +4472,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -4501,7 +4505,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4534,7 +4538,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4567,7 +4571,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4600,7 +4604,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4633,7 +4637,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4666,7 +4670,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4699,7 +4703,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -4732,7 +4736,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -4765,7 +4769,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -4798,7 +4802,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -4831,7 +4835,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -4864,7 +4868,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -4897,7 +4901,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -4930,7 +4934,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -4963,7 +4967,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -4996,7 +5000,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -5029,7 +5033,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5062,7 +5066,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5095,7 +5099,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="275.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" ht="285" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5128,7 +5132,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5161,7 +5165,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5194,7 +5198,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5227,7 +5231,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -5260,7 +5264,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -5293,7 +5297,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -5326,7 +5330,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -5359,7 +5363,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="87" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -5392,7 +5396,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -5425,7 +5429,7 @@
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -5458,7 +5462,7 @@
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -5491,7 +5495,7 @@
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -5524,7 +5528,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5557,7 +5561,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5590,7 +5594,7 @@
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -5623,7 +5627,7 @@
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -5656,7 +5660,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -5689,7 +5693,7 @@
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="174" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -5722,7 +5726,7 @@
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -5755,7 +5759,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -5788,7 +5792,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="333.5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" ht="345" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -5821,7 +5825,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -5854,7 +5858,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -5887,7 +5891,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -5920,7 +5924,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5955,7 +5959,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -5988,7 +5992,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -6023,7 +6027,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -6058,7 +6062,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -6091,7 +6095,7 @@
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -6126,7 +6130,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -6159,7 +6163,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -6192,7 +6196,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -6225,7 +6229,7 @@
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -6258,7 +6262,7 @@
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -6291,7 +6295,7 @@
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -6324,7 +6328,7 @@
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -6359,7 +6363,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -6392,7 +6396,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -6425,7 +6429,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -6458,7 +6462,7 @@
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -6491,7 +6495,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -6524,7 +6528,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -6557,7 +6561,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
@@ -6588,7 +6592,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>170</v>
       </c>
@@ -6621,7 +6625,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>170</v>
       </c>
@@ -6654,7 +6658,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>170</v>
       </c>
@@ -6687,7 +6691,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>170</v>
       </c>
@@ -6720,7 +6724,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -6753,7 +6757,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>170</v>
       </c>
@@ -6786,7 +6790,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>170</v>
       </c>
@@ -6819,7 +6823,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -6852,7 +6856,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>170</v>
       </c>
@@ -6885,7 +6889,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -6918,7 +6922,7 @@
       </c>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>170</v>
       </c>
@@ -6951,7 +6955,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>170</v>
       </c>
@@ -6984,7 +6988,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -7017,7 +7021,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -7050,7 +7054,7 @@
       </c>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>170</v>
       </c>
@@ -7083,7 +7087,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>170</v>
       </c>
@@ -7099,7 +7103,9 @@
       <c r="E84" s="37">
         <v>44635</v>
       </c>
-      <c r="F84" s="38"/>
+      <c r="F84" s="38" t="s">
+        <v>257</v>
+      </c>
       <c r="G84" s="14">
         <v>44649</v>
       </c>
@@ -7108,7 +7114,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -7139,7 +7145,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -7164,7 +7170,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -7195,7 +7201,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -7222,7 +7228,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>170</v>
       </c>
@@ -7253,7 +7259,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>170</v>
       </c>
@@ -7284,7 +7290,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>170</v>
       </c>
@@ -7306,12 +7312,16 @@
       <c r="G91" s="14">
         <v>44649</v>
       </c>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
+      <c r="H91" s="11">
+        <v>44648</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="29" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>170</v>
       </c>
@@ -7342,7 +7352,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>246</v>
       </c>
@@ -7388,15 +7398,15 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1727200</xdr:colOff>
+                <xdr:colOff>1729740</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>50800</xdr:rowOff>
+                <xdr:rowOff>53340</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2216150</xdr:colOff>
+                <xdr:colOff>2217420</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>330200</xdr:rowOff>
+                <xdr:rowOff>327660</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7413,15 +7423,15 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2311400</xdr:colOff>
+                <xdr:colOff>2308860</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>222250</xdr:rowOff>
+                <xdr:rowOff>220980</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>2933700</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>539750</xdr:rowOff>
+                <xdr:rowOff>541020</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7443,19 +7453,19 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="20" width="5.6328125" customWidth="1"/>
-    <col min="21" max="21" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="5.6640625" customWidth="1"/>
+    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>235</v>
       </c>
@@ -7487,7 +7497,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>233</v>
       </c>
@@ -7540,7 +7550,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>161</v>
       </c>
@@ -7575,7 +7585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="30">
         <v>44575</v>
       </c>
@@ -7606,7 +7616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="30">
         <v>44587</v>
       </c>
@@ -7637,7 +7647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>44589</v>
       </c>
@@ -7668,7 +7678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="30">
         <v>44615</v>
       </c>
@@ -7707,7 +7717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
         <v>44635</v>
       </c>
@@ -7740,7 +7750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="30">
         <v>44638</v>
       </c>
@@ -7771,7 +7781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
         <v>169</v>
       </c>
@@ -7828,7 +7838,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>220</v>
       </c>
@@ -7870,7 +7880,7 @@
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>245</v>
       </c>
@@ -7948,7 +7958,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="str">
         <f t="shared" ref="A18:S18" si="1">A6</f>
         <v>2022/2/8、2022/2/11</v>
@@ -8030,7 +8040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="32">
         <f t="shared" ref="A19:S19" si="2">A7</f>
         <v>44575</v>
@@ -8112,7 +8122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
         <f t="shared" ref="A20:S20" si="4">A8</f>
         <v>44587</v>
@@ -8194,7 +8204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="32">
         <f t="shared" ref="A21:S21" si="5">A9</f>
         <v>44589</v>
@@ -8276,7 +8286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="32">
         <f t="shared" ref="A22:S22" si="6">A10</f>
         <v>44615</v>
@@ -8358,7 +8368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="32">
         <f t="shared" ref="A23:S23" si="7">A11</f>
         <v>44635</v>
@@ -8440,7 +8450,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="32">
         <f t="shared" ref="A24:S24" si="8">A12</f>
         <v>44638</v>
@@ -8519,7 +8529,7 @@
       </c>
       <c r="T24" s="25"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="str">
         <f t="shared" ref="A25:S25" si="9">A13</f>
         <v>總計</v>
@@ -8609,6 +8619,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -8722,33 +8747,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8769,9 +8771,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/29 週二
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB52625A-28F9-4E36-A48D-547D31CA67BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA1529B-B881-424C-9700-A05AC9E18C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="263">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1211,11 +1211,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.授權辦理事項：三個選項應為■查詢■覆核■其他，請將系統第一個選項審查更改為查詢。
-2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>銷號欄開放輸入</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1228,18 +1223,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>聯徵MU1爆送：L8950、L8350、L8351</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>新增連動[L2902 保證人保證資料查詢]與[L4960 火險保費資料查詢(By客戶)]</t>
   </si>
   <si>
     <t>入帳日與金額可修改,金額依入帳日預設可修改</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>問佩瑜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1253,6 +1240,43 @@
   </si>
   <si>
     <t>增加按鈕連動相關交易</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L8081AML定審通知處理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、附件上傳後，當下列印資料，有附件資料措述，但無法看到附件內容。
+2、後續查詢內容，無查詢到有附件上傳記錄資料。
+3、通知內容僅顯示最後一筆通知，歷史記錄及之前如有附件，要如何得知。
+4、測試資料僅高、低有資料，問題相同，中風險無資料無法測試。
+5、AML定審資料為ａｍｌ系統發動，無法確認後續轉檔是否正確。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施美娟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L6705聯徵報送-地區別資料維護</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鄧雪美</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增地區別畫面：部室代號非為必要欄位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L8350聯徵MU1報送</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.授權辦理事項：三個選項應為：查詢、覆核、其他，請將系統第一個選項審查更改為查詢。
+2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1263,7 +1287,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1334,13 +1358,6 @@
       <color theme="1"/>
       <name val="標楷體"/>
       <family val="4"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
@@ -1421,7 +1438,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1500,9 +1517,6 @@
     <xf numFmtId="9" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1">
       <alignment vertical="center"/>
     </xf>
@@ -1539,10 +1553,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2484,15 +2498,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1729740</xdr:colOff>
+          <xdr:colOff>1727200</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>50800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2217420</xdr:colOff>
+          <xdr:colOff>2216150</xdr:colOff>
           <xdr:row>85</xdr:row>
-          <xdr:rowOff>327660</xdr:rowOff>
+          <xdr:rowOff>330200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2539,15 +2553,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2308860</xdr:colOff>
+          <xdr:colOff>2311400</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>220980</xdr:rowOff>
+          <xdr:rowOff>222250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>2933700</xdr:colOff>
           <xdr:row>83</xdr:row>
-          <xdr:rowOff>541020</xdr:rowOff>
+          <xdr:rowOff>539750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2593,7 +2607,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44645.46858645833" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="93" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44649.523440046294" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="95" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K1048576" sheet="User審查意見彙整"/>
   </cacheSource>
@@ -2611,7 +2625,7 @@
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
     <cacheField name="意見收到日" numFmtId="14">
-      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2022-01-14T00:00:00" maxDate="2022-03-19T00:00:00" count="8">
+      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2022-01-14T00:00:00" maxDate="2022-03-30T00:00:00" count="9">
         <d v="2022-01-14T00:00:00"/>
         <d v="2022-01-26T00:00:00"/>
         <d v="2022-01-28T00:00:00"/>
@@ -2619,6 +2633,7 @@
         <d v="2022-02-23T00:00:00"/>
         <d v="2022-03-15T00:00:00"/>
         <d v="2022-03-18T00:00:00"/>
+        <d v="2022-03-29T00:00:00"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -2626,7 +2641,7 @@
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
     <cacheField name="預計完成日" numFmtId="14">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-30T00:00:00" count="13">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-30T00:00:00" count="14">
         <d v="2022-01-21T00:00:00"/>
         <d v="2022-02-09T00:00:00"/>
         <d v="2022-02-11T00:00:00"/>
@@ -2638,6 +2653,7 @@
         <d v="2022-03-16T00:00:00"/>
         <d v="2022-03-29T00:00:00"/>
         <d v="2022-03-23T00:00:00"/>
+        <d v="2022-03-25T00:00:00"/>
         <d v="2022-03-21T00:00:00"/>
         <m/>
       </sharedItems>
@@ -2660,7 +2676,7 @@
       </fieldGroup>
     </cacheField>
     <cacheField name="意見回覆日" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-23T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-29T00:00:00"/>
     </cacheField>
     <cacheField name="回覆狀態" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -2681,7 +2697,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="93">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="95">
   <r>
     <s v="邵淑微"/>
     <n v="1"/>
@@ -3754,7 +3770,7 @@
     <s v="L2631清償作業"/>
     <s v="呈現畫面資訊不夠：是否可以比照舊有的畫面顯示，如附件_x000a_押品地址就秀最後一個額度"/>
     <x v="5"/>
-    <m/>
+    <s v="增加按鈕連動相關交易"/>
     <x v="9"/>
     <m/>
     <m/>
@@ -3806,8 +3822,8 @@
     <s v="L2631清償作業"/>
     <s v="當初有提到可以多額度選取，請問如果要選擇1跟4額度時，要如何處理?"/>
     <x v="5"/>
-    <s v="問佩瑜"/>
-    <x v="9"/>
+    <m/>
+    <x v="11"/>
     <m/>
     <m/>
     <m/>
@@ -3820,7 +3836,7 @@
     <s v="是否有判斷，同押品是否同時要結清或是餘額為0，才可領取清償證明。"/>
     <x v="5"/>
     <s v="判斷擔保品需全部結案才可領取清償證明"/>
-    <x v="11"/>
+    <x v="12"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3833,7 +3849,7 @@
     <s v="關於申請日期，應為系統之日曆日，非會計日"/>
     <x v="5"/>
     <s v="已修正"/>
-    <x v="11"/>
+    <x v="12"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3846,9 +3862,9 @@
     <s v="未結清時，修改金額，而非修改入帳日"/>
     <x v="5"/>
     <s v="入帳日與金額可修改,金額依入帳日預設可修改"/>
-    <x v="9"/>
-    <m/>
-    <m/>
+    <x v="11"/>
+    <d v="2022-03-28T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3859,7 +3875,7 @@
     <s v="已結清時，銷號欄要可輸入"/>
     <x v="5"/>
     <s v="銷號欄開放輸入"/>
-    <x v="11"/>
+    <x v="12"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3868,10 +3884,10 @@
   <r>
     <s v="程慧娟"/>
     <n v="1"/>
-    <s v="聯徵MU1爆送：L8950、L8350、L8351"/>
-    <s v="1.授權辦理事項：三個選項應為■查詢■覆核■其他，請將系統第一個選項審查更改為查詢。_x000a_2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。"/>
+    <s v="L8350聯徵MU1報送"/>
+    <s v="1.授權辦理事項：三個選項應為：查詢、覆核、其他，請將系統第一個選項審查更改為查詢。_x000a_2.分行代號：因為原放款管理課已撤銷，請將原CR06放款管理課刪除，加入CR05放款服務課。"/>
     <x v="6"/>
-    <s v="1.程式調整_x000a_2.以代碼交易調整"/>
+    <s v="1.URS、程式調整_x000a_2.以代碼交易調整"/>
     <x v="5"/>
     <d v="2022-03-21T00:00:00"/>
     <s v="已完成"/>
@@ -3879,13 +3895,39 @@
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <s v="施美娟"/>
+    <n v="1"/>
+    <s v="L8081AML定審通知處理"/>
+    <s v="1、附件上傳後，當下列印資料，有附件資料措述，但無法看到附件內容。_x000a_2、後續查詢內容，無查詢到有附件上傳記錄資料。_x000a_3、通知內容僅顯示最後一筆通知，歷史記錄及之前如有附件，要如何得知。_x000a_4、測試資料僅高、低有資料，問題相同，中風險無資料無法測試。_x000a_5、AML定審資料為ａｍｌ系統發動，無法確認後續轉檔是否正確。"/>
     <x v="7"/>
     <m/>
-    <x v="12"/>
+    <x v="13"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="鄧雪美"/>
+    <n v="2"/>
+    <s v="L6705聯徵報送-地區別資料維護"/>
+    <s v="新增地區別畫面：部室代號非為必要欄位"/>
+    <x v="7"/>
+    <m/>
+    <x v="13"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="8"/>
+    <m/>
+    <x v="13"/>
     <m/>
     <m/>
     <m/>
@@ -3895,7 +3937,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:S13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -3903,15 +3945,16 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="9">
+      <items count="10">
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="4"/>
         <item x="5"/>
+        <item h="1" x="8"/>
+        <item x="6"/>
         <item h="1" x="7"/>
-        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -4314,31 +4357,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
+      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="44.6328125" style="16" customWidth="1"/>
     <col min="5" max="5" width="13" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>162</v>
       </c>
@@ -4373,7 +4416,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4406,7 +4449,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -4439,7 +4482,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4472,7 +4515,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -4505,7 +4548,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -4538,7 +4581,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4571,7 +4614,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -4604,7 +4647,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -4637,7 +4680,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -4670,7 +4713,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -4703,7 +4746,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -4736,7 +4779,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -4769,7 +4812,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -4802,7 +4845,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -4835,7 +4878,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -4868,7 +4911,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -4901,7 +4944,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -4934,7 +4977,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -4967,7 +5010,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -5000,7 +5043,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -5033,7 +5076,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5066,7 +5109,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="409.5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5099,7 +5142,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="285" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="275.5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5132,7 +5175,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5165,7 +5208,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="217.5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5198,7 +5241,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5231,7 +5274,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -5264,7 +5307,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -5297,7 +5340,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -5330,7 +5373,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -5363,7 +5406,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="87" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -5396,7 +5439,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -5429,7 +5472,7 @@
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -5462,7 +5505,7 @@
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -5495,7 +5538,7 @@
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -5528,7 +5571,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="101.5" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -5561,7 +5604,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="159.5" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -5594,7 +5637,7 @@
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -5627,7 +5670,7 @@
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -5660,7 +5703,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -5693,7 +5736,7 @@
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="174" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -5726,7 +5769,7 @@
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -5759,7 +5802,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -5792,7 +5835,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="345" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="333.5" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -5825,7 +5868,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -5858,7 +5901,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -5891,7 +5934,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="72.5" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -5924,7 +5967,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5959,7 +6002,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -5992,7 +6035,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -6027,7 +6070,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -6062,7 +6105,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -6095,7 +6138,7 @@
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -6130,7 +6173,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -6163,7 +6206,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -6196,7 +6239,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -6229,7 +6272,7 @@
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -6262,7 +6305,7 @@
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -6295,7 +6338,7 @@
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -6328,7 +6371,7 @@
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -6363,7 +6406,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -6396,7 +6439,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -6429,7 +6472,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -6462,7 +6505,7 @@
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -6495,7 +6538,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -6528,7 +6571,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="135" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="130.5" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -6561,7 +6604,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
@@ -6592,7 +6635,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>170</v>
       </c>
@@ -6625,7 +6668,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>170</v>
       </c>
@@ -6658,7 +6701,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>170</v>
       </c>
@@ -6691,7 +6734,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>170</v>
       </c>
@@ -6724,7 +6767,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -6757,7 +6800,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>170</v>
       </c>
@@ -6790,7 +6833,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>170</v>
       </c>
@@ -6823,7 +6866,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -6856,7 +6899,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>170</v>
       </c>
@@ -6889,7 +6932,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -6922,7 +6965,7 @@
       </c>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>170</v>
       </c>
@@ -6955,7 +6998,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>170</v>
       </c>
@@ -6988,7 +7031,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -7021,7 +7064,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -7054,7 +7097,7 @@
       </c>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>170</v>
       </c>
@@ -7087,7 +7130,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>170</v>
       </c>
@@ -7097,14 +7140,14 @@
       <c r="C84" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D84" s="36" t="s">
+      <c r="D84" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="E84" s="37">
+      <c r="E84" s="36">
         <v>44635</v>
       </c>
-      <c r="F84" s="38" t="s">
-        <v>257</v>
+      <c r="F84" s="37" t="s">
+        <v>254</v>
       </c>
       <c r="G84" s="14">
         <v>44649</v>
@@ -7114,7 +7157,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -7131,7 +7174,7 @@
         <v>44635</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G85" s="14">
         <v>44643</v>
@@ -7145,7 +7188,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -7155,13 +7198,13 @@
       <c r="C86" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D86" s="36" t="s">
+      <c r="D86" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="E86" s="37">
+      <c r="E86" s="36">
         <v>44635</v>
       </c>
-      <c r="F86" s="38"/>
+      <c r="F86" s="37"/>
       <c r="G86" s="14">
         <v>44649</v>
       </c>
@@ -7170,7 +7213,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -7187,7 +7230,7 @@
         <v>44635</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G87" s="14">
         <v>44643</v>
@@ -7201,7 +7244,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -7211,24 +7254,22 @@
       <c r="C88" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D88" s="36" t="s">
+      <c r="D88" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="E88" s="37">
+      <c r="E88" s="36">
         <v>44635</v>
       </c>
-      <c r="F88" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="G88" s="14">
-        <v>44649</v>
+      <c r="F88" s="37"/>
+      <c r="G88" s="39">
+        <v>44645</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>170</v>
       </c>
@@ -7238,14 +7279,14 @@
       <c r="C89" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="36" t="s">
+      <c r="D89" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="E89" s="37">
+      <c r="E89" s="36">
         <v>44635</v>
       </c>
-      <c r="F89" s="38" t="s">
-        <v>255</v>
+      <c r="F89" s="37" t="s">
+        <v>252</v>
       </c>
       <c r="G89" s="14">
         <v>44641</v>
@@ -7259,7 +7300,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>170</v>
       </c>
@@ -7276,7 +7317,7 @@
         <v>44635</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G90" s="14">
         <v>44641</v>
@@ -7290,7 +7331,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>170</v>
       </c>
@@ -7300,17 +7341,17 @@
       <c r="C91" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D91" s="39" t="s">
+      <c r="D91" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="E91" s="37">
+      <c r="E91" s="36">
         <v>44635</v>
       </c>
-      <c r="F91" s="38" t="s">
-        <v>253</v>
+      <c r="F91" s="37" t="s">
+        <v>251</v>
       </c>
       <c r="G91" s="14">
-        <v>44649</v>
+        <v>44645</v>
       </c>
       <c r="H91" s="11">
         <v>44648</v>
@@ -7321,7 +7362,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="29" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>170</v>
       </c>
@@ -7331,14 +7372,14 @@
       <c r="C92" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D92" s="26" t="s">
+      <c r="D92" s="6" t="s">
         <v>230</v>
       </c>
       <c r="E92" s="13">
         <v>44635</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G92" s="14">
         <v>44641</v>
@@ -7352,7 +7393,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="58" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>246</v>
       </c>
@@ -7360,16 +7401,16 @@
         <v>1</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="E93" s="13">
         <v>44638</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G93" s="14">
         <v>44642</v>
@@ -7382,6 +7423,52 @@
       </c>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
+    </row>
+    <row r="94" spans="1:11" ht="145" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E94" s="13">
+        <v>44649</v>
+      </c>
+      <c r="F94" s="2"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+    </row>
+    <row r="95" spans="1:11" ht="58" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B95" s="2">
+        <v>2</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E95" s="13">
+        <v>44649</v>
+      </c>
+      <c r="F95" s="2"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K93" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -7398,15 +7485,15 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1729740</xdr:colOff>
+                <xdr:colOff>1727200</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>53340</xdr:rowOff>
+                <xdr:rowOff>50800</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2217420</xdr:colOff>
+                <xdr:colOff>2216150</xdr:colOff>
                 <xdr:row>85</xdr:row>
-                <xdr:rowOff>327660</xdr:rowOff>
+                <xdr:rowOff>330200</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7423,15 +7510,15 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>2308860</xdr:colOff>
+                <xdr:colOff>2311400</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>220980</xdr:rowOff>
+                <xdr:rowOff>222250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>2933700</xdr:colOff>
                 <xdr:row>83</xdr:row>
-                <xdr:rowOff>541020</xdr:rowOff>
+                <xdr:rowOff>539750</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -7449,23 +7536,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E69748B-F013-4C3D-B545-0E0A517A1BB7}">
   <dimension ref="A3:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="20" width="5.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6328125" customWidth="1"/>
+    <col min="21" max="21" width="28.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B3" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>235</v>
       </c>
@@ -7497,8 +7601,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A5" s="26" t="s">
         <v>233</v>
       </c>
       <c r="B5" t="s">
@@ -7550,401 +7654,401 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A6" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28">
         <v>22</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>22</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="28">
         <v>1</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="28">
         <v>1</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29">
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28">
         <v>23</v>
       </c>
-      <c r="S6" s="29">
+      <c r="S6" s="28">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A7" s="29">
         <v>44575</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>21</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>21</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28">
         <v>21</v>
       </c>
-      <c r="S7" s="29">
+      <c r="S7" s="28">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A8" s="29">
         <v>44587</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28">
         <v>3</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>3</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29">
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28">
         <v>3</v>
       </c>
-      <c r="S8" s="29">
+      <c r="S8" s="28">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A9" s="29">
         <v>44589</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28">
         <v>19</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>19</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29">
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28">
         <v>19</v>
       </c>
-      <c r="S9" s="29">
+      <c r="S9" s="28">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A10" s="29">
         <v>44615</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28">
         <v>3</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="28">
         <v>3</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="28">
         <v>12</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="28">
         <v>12</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="28">
         <v>1</v>
       </c>
-      <c r="O10" s="29">
+      <c r="O10" s="28">
         <v>1</v>
       </c>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29">
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28">
         <v>16</v>
       </c>
-      <c r="S10" s="29">
+      <c r="S10" s="28">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A11" s="29">
         <v>44635</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29">
-        <v>5</v>
-      </c>
-      <c r="O11" s="29">
-        <v>5</v>
-      </c>
-      <c r="P11" s="29">
-        <v>4</v>
-      </c>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28">
+        <v>7</v>
+      </c>
+      <c r="O11" s="28">
+        <v>6</v>
+      </c>
+      <c r="P11" s="28">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28">
         <v>9</v>
       </c>
-      <c r="S11" s="29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="S11" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A12" s="29">
         <v>44638</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28">
         <v>1</v>
       </c>
-      <c r="O12" s="29">
+      <c r="O12" s="28">
         <v>1</v>
       </c>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29">
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28">
         <v>1</v>
       </c>
-      <c r="S12" s="29">
+      <c r="S12" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A13" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="28">
         <v>21</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>21</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>22</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="28">
         <v>22</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="28">
         <v>22</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="28">
         <v>22</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="28">
         <v>1</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="28">
         <v>1</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="28">
         <v>3</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="28">
         <v>3</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="28">
         <v>12</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="28">
         <v>12</v>
       </c>
-      <c r="N13" s="29">
-        <v>7</v>
-      </c>
-      <c r="O13" s="29">
-        <v>7</v>
-      </c>
-      <c r="P13" s="29">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29">
+      <c r="N13" s="28">
+        <v>9</v>
+      </c>
+      <c r="O13" s="28">
+        <v>8</v>
+      </c>
+      <c r="P13" s="28">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28">
         <v>92</v>
       </c>
-      <c r="S13" s="29">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="S13" s="28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="33">
         <v>44583</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34">
+      <c r="C16" s="33"/>
+      <c r="D16" s="33">
         <v>44603</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34">
+      <c r="E16" s="33"/>
+      <c r="F16" s="33">
         <v>44610</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34">
+      <c r="G16" s="33"/>
+      <c r="H16" s="33">
         <v>44617</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34">
+      <c r="I16" s="33"/>
+      <c r="J16" s="33">
         <v>44631</v>
       </c>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34">
+      <c r="K16" s="33"/>
+      <c r="L16" s="33">
         <v>44638</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34">
+      <c r="M16" s="33"/>
+      <c r="N16" s="33">
         <v>44645</v>
       </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34">
+      <c r="O16" s="33"/>
+      <c r="P16" s="33">
         <v>44651</v>
       </c>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="33" t="s">
+      <c r="Q16" s="33"/>
+      <c r="R16" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A17" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="B17" s="35" t="str">
+      <c r="B17" s="34" t="str">
         <f t="shared" ref="B17:Q17" si="0">B5</f>
         <v>預計</v>
       </c>
-      <c r="C17" s="35" t="str">
+      <c r="C17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="D17" s="35" t="str">
+      <c r="D17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="E17" s="35" t="str">
+      <c r="E17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="F17" s="35" t="str">
+      <c r="F17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="G17" s="35" t="str">
+      <c r="G17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="H17" s="35" t="str">
+      <c r="H17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="I17" s="35" t="str">
+      <c r="I17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="J17" s="35" t="str">
+      <c r="J17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="K17" s="35" t="str">
+      <c r="K17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="L17" s="35" t="str">
+      <c r="L17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="M17" s="35" t="str">
+      <c r="M17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="N17" s="35" t="str">
+      <c r="N17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="O17" s="35" t="str">
+      <c r="O17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="P17" s="35" t="str">
+      <c r="P17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="Q17" s="35" t="str">
+      <c r="Q17" s="34" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
@@ -7958,8 +8062,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="str">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A18" s="38" t="str">
         <f t="shared" ref="A18:S18" si="1">A6</f>
         <v>2022/2/8、2022/2/11</v>
       </c>
@@ -8040,8 +8144,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="32">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A19" s="31">
         <f t="shared" ref="A19:S19" si="2">A7</f>
         <v>44575</v>
       </c>
@@ -8122,8 +8226,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="32">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A20" s="31">
         <f t="shared" ref="A20:S20" si="4">A8</f>
         <v>44587</v>
       </c>
@@ -8204,8 +8308,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="32">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A21" s="31">
         <f t="shared" ref="A21:S21" si="5">A9</f>
         <v>44589</v>
       </c>
@@ -8286,8 +8390,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="32">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A22" s="31">
         <f t="shared" ref="A22:S22" si="6">A10</f>
         <v>44615</v>
       </c>
@@ -8368,8 +8472,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="32">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A23" s="31">
         <f t="shared" ref="A23:S23" si="7">A11</f>
         <v>44635</v>
       </c>
@@ -8423,15 +8527,15 @@
       </c>
       <c r="N23" s="17">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O23" s="17">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P23" s="17">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="17">
         <f t="shared" si="7"/>
@@ -8443,15 +8547,15 @@
       </c>
       <c r="S23" s="18">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T23" s="25">
         <f t="shared" si="3"/>
-        <v>0.55555555555555558</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="32">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A24" s="31">
         <f t="shared" ref="A24:S24" si="8">A12</f>
         <v>44638</v>
       </c>
@@ -8529,72 +8633,72 @@
       </c>
       <c r="T24" s="25"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="str">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A25" s="34" t="str">
         <f t="shared" ref="A25:S25" si="9">A13</f>
         <v>總計</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="34">
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="34">
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="34">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="34">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="34">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="G25" s="35">
+      <c r="G25" s="34">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="34">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="I25" s="35">
+      <c r="I25" s="34">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J25" s="35">
+      <c r="J25" s="34">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="34">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="L25" s="35">
+      <c r="L25" s="34">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="M25" s="35">
+      <c r="M25" s="34">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="N25" s="35">
+      <c r="N25" s="34">
         <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="O25" s="35">
+        <v>9</v>
+      </c>
+      <c r="O25" s="34">
         <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="P25" s="35">
+        <v>8</v>
+      </c>
+      <c r="P25" s="34">
         <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="Q25" s="35">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="34">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -8604,11 +8708,11 @@
       </c>
       <c r="S25" s="18">
         <f t="shared" si="9"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="T25" s="25">
         <f t="shared" si="3"/>
-        <v>0.95652173913043481</v>
+        <v>0.96739130434782605</v>
       </c>
     </row>
   </sheetData>
@@ -8619,21 +8723,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -8747,10 +8836,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8771,17 +8883,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/03/30 週三
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,21 +5,21 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D2E7E0-A0D0-440E-973B-11B4FF584F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217A29E0-84A8-4721-B4E0-178214A1C2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
   <sheets>
     <sheet name="User審查意見彙整" sheetId="7" r:id="rId1"/>
     <sheet name="工作表2" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">User審查意見彙整!$A$1:$K$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">User審查意見彙整!$A$1:$K$96</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
@@ -32,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="269">
   <si>
     <t>章節及說明</t>
   </si>
@@ -1285,6 +1286,29 @@
   </si>
   <si>
     <t>需登打兩次交易額度1與額度4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L3002撥款明細資料查詢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.欄位:戶況：為何有"展期"的戶況
+2.無欄位：需有"撥款金額"跟"企金別"的欄位
+3.欄位:展期件：匯出試算表後無此欄位，如附件[L3002]撥款明細資料_20220322_112048
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.賴桑
+2.新增欄位
+3.展期件為按鈕,在問小潘是否能顯示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3項會提供測試說明,也可當面說明
+4.L8082查詢109/07/05有資料
+5.目前測試資料為人工造的資料,建議於平測由AML系統匯入,王行確認</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1362,13 +1386,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="標楷體"/>
       <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="標楷體"/>
@@ -1446,7 +1471,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1480,9 +1505,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1497,12 +1519,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1522,36 +1538,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1561,15 +1547,313 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="標楷體"/>
+        <family val="4"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2608,11 +2892,66 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>2720340</xdr:colOff>
+          <xdr:row>95</xdr:row>
+          <xdr:rowOff>632460</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>3009900</xdr:colOff>
+          <xdr:row>95</xdr:row>
+          <xdr:rowOff>906780</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Object 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44649.523440046294" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="95" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Susan Ho" refreshedDate="44649.779659490741" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="96" xr:uid="{A180C8E4-AC99-4C76-9656-5A1735AF9F43}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K1048576" sheet="User審查意見彙整"/>
   </cacheSource>
@@ -2646,7 +2985,7 @@
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
     <cacheField name="預計完成日" numFmtId="14">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-30T00:00:00" count="14">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-04-01T00:00:00" count="15">
         <d v="2022-01-21T00:00:00"/>
         <d v="2022-02-09T00:00:00"/>
         <d v="2022-02-11T00:00:00"/>
@@ -2658,9 +2997,10 @@
         <d v="2022-03-16T00:00:00"/>
         <d v="2022-03-29T00:00:00"/>
         <d v="2022-03-23T00:00:00"/>
+        <d v="2022-03-21T00:00:00"/>
         <d v="2022-03-25T00:00:00"/>
-        <d v="2022-03-21T00:00:00"/>
         <m/>
+        <d v="2022-03-31T00:00:00"/>
       </sharedItems>
       <fieldGroup base="6">
         <rangePr autoStart="0" autoEnd="0" groupBy="days" startDate="2022-01-22T00:00:00" endDate="2022-04-02T00:00:00" groupInterval="7"/>
@@ -2681,7 +3021,7 @@
       </fieldGroup>
     </cacheField>
     <cacheField name="意見回覆日" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-29T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2022-01-21T00:00:00" maxDate="2022-03-30T00:00:00"/>
     </cacheField>
     <cacheField name="回覆狀態" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -2702,7 +3042,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="95">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="96">
   <r>
     <s v="邵淑微"/>
     <n v="1"/>
@@ -3777,8 +4117,8 @@
     <x v="5"/>
     <s v="增加按鈕連動相關交易"/>
     <x v="9"/>
-    <m/>
-    <m/>
+    <d v="2022-03-29T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3801,10 +4141,10 @@
     <s v="L2631清償作業"/>
     <s v="登錄後列印文件：如附件"/>
     <x v="5"/>
-    <m/>
+    <s v="按鈕連動相關交易可另外列印"/>
     <x v="9"/>
-    <m/>
-    <m/>
+    <d v="2022-03-29T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3827,10 +4167,10 @@
     <s v="L2631清償作業"/>
     <s v="當初有提到可以多額度選取，請問如果要選擇1跟4額度時，要如何處理?"/>
     <x v="5"/>
-    <m/>
-    <x v="11"/>
-    <m/>
-    <m/>
+    <s v="需登打兩次交易額度1與額度4"/>
+    <x v="9"/>
+    <d v="2022-03-29T00:00:00"/>
+    <s v="已完成"/>
     <m/>
     <m/>
   </r>
@@ -3841,7 +4181,7 @@
     <s v="是否有判斷，同押品是否同時要結清或是餘額為0，才可領取清償證明。"/>
     <x v="5"/>
     <s v="判斷擔保品需全部結案才可領取清償證明"/>
-    <x v="12"/>
+    <x v="11"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3854,7 +4194,7 @@
     <s v="關於申請日期，應為系統之日曆日，非會計日"/>
     <x v="5"/>
     <s v="已修正"/>
-    <x v="12"/>
+    <x v="11"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3867,7 +4207,7 @@
     <s v="未結清時，修改金額，而非修改入帳日"/>
     <x v="5"/>
     <s v="入帳日與金額可修改,金額依入帳日預設可修改"/>
-    <x v="11"/>
+    <x v="12"/>
     <d v="2022-03-28T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3880,7 +4220,7 @@
     <s v="已結清時，銷號欄要可輸入"/>
     <x v="5"/>
     <s v="銷號欄開放輸入"/>
-    <x v="12"/>
+    <x v="11"/>
     <d v="2022-03-22T00:00:00"/>
     <s v="已完成"/>
     <m/>
@@ -3919,7 +4259,20 @@
     <s v="新增地區別畫面：部室代號非為必要欄位"/>
     <x v="7"/>
     <m/>
-    <x v="13"/>
+    <x v="14"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="蔡珮瑜"/>
+    <n v="3"/>
+    <s v="L3002撥款明細資料查詢"/>
+    <s v="1.欄位:戶況：為何有&quot;展期&quot;的戶況_x000a_2.無欄位：需有&quot;撥款金額&quot;跟&quot;企金別&quot;的欄位_x000a_3.欄位:展期件：匯出試算表後無此欄位，如附件[L3002]撥款明細資料_20220322_112048_x000a_"/>
+    <x v="7"/>
+    <s v="1.賴桑_x000a_2.新增欄位_x000a_3.展期件為按鈕,在問小潘是否能顯示"/>
+    <x v="14"/>
     <m/>
     <m/>
     <m/>
@@ -3943,7 +4296,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{59393228-44BF-4CA9-BF68-DEE573318B19}" name="樞紐分析表2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:S13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <location ref="A3:S14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -3959,7 +4312,7 @@
         <item x="5"/>
         <item h="1" x="8"/>
         <item x="6"/>
-        <item h="1" x="7"/>
+        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3989,7 +4342,7 @@
   <rowFields count="1">
     <field x="4"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x/>
     </i>
@@ -4010,6 +4363,9 @@
     </i>
     <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -4087,6 +4443,346 @@
     <dataField name="預計" fld="6" subtotal="count" baseField="4" baseItem="0"/>
     <dataField name="實際" fld="7" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
+  <formats count="40">
+    <format dxfId="39">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="38">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="36">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="35">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="34">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="33">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="8">
+            <x v="0"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea field="6" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea field="6" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="17">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="8">
+            <x v="0"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="6" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea field="6" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -4362,24 +5058,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H88" sqref="H88"/>
+      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="16" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="15" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.77734375" style="1" customWidth="1"/>
@@ -4405,10 +5101,10 @@
       <c r="F1" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="26" t="s">
         <v>36</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -4434,13 +5130,13 @@
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>44575</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>44582</v>
       </c>
       <c r="H2" s="7">
@@ -4467,13 +5163,13 @@
       <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>44575</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>44582</v>
       </c>
       <c r="H3" s="7">
@@ -4500,13 +5196,13 @@
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>44575</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>44582</v>
       </c>
       <c r="H4" s="7">
@@ -4533,13 +5229,13 @@
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>44575</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>44582</v>
       </c>
       <c r="H5" s="7">
@@ -4566,13 +5262,13 @@
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>44575</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>44582</v>
       </c>
       <c r="H6" s="7">
@@ -4599,13 +5295,13 @@
       <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>44575</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>44582</v>
       </c>
       <c r="H7" s="7">
@@ -4632,13 +5328,13 @@
       <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>44575</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>44582</v>
       </c>
       <c r="H8" s="7">
@@ -4665,13 +5361,13 @@
       <c r="D9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>44575</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>44582</v>
       </c>
       <c r="H9" s="7">
@@ -4698,13 +5394,13 @@
       <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>44575</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>44582</v>
       </c>
       <c r="H10" s="7">
@@ -4731,13 +5427,13 @@
       <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>44575</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>44582</v>
       </c>
       <c r="H11" s="7">
@@ -4764,13 +5460,13 @@
       <c r="D12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <v>44575</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>44582</v>
       </c>
       <c r="H12" s="7">
@@ -4797,13 +5493,13 @@
       <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>44575</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>44582</v>
       </c>
       <c r="H13" s="7">
@@ -4830,13 +5526,13 @@
       <c r="D14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>44575</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>44582</v>
       </c>
       <c r="H14" s="7">
@@ -4863,13 +5559,13 @@
       <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>44575</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>44582</v>
       </c>
       <c r="H15" s="7">
@@ -4896,13 +5592,13 @@
       <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>44575</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>44582</v>
       </c>
       <c r="H16" s="7">
@@ -4929,13 +5625,13 @@
       <c r="D17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>44575</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>44582</v>
       </c>
       <c r="H17" s="7">
@@ -4962,13 +5658,13 @@
       <c r="D18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>44575</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>44582</v>
       </c>
       <c r="H18" s="7">
@@ -4995,13 +5691,13 @@
       <c r="D19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>44575</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>44582</v>
       </c>
       <c r="H19" s="7">
@@ -5028,13 +5724,13 @@
       <c r="D20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>44575</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>44582</v>
       </c>
       <c r="H20" s="7">
@@ -5061,13 +5757,13 @@
       <c r="D21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>44575</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>44582</v>
       </c>
       <c r="H21" s="7">
@@ -5094,13 +5790,13 @@
       <c r="D22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <v>44575</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>44582</v>
       </c>
       <c r="H22" s="7">
@@ -5124,19 +5820,19 @@
       <c r="C23" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>44587</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <v>44601</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="27">
         <v>44588</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -5157,19 +5853,19 @@
       <c r="C24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="12">
         <v>44587</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="12">
         <v>44601</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="27">
         <v>44588</v>
       </c>
       <c r="I24" s="2" t="s">
@@ -5190,19 +5886,19 @@
       <c r="C25" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <v>44587</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>44601</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="27">
         <v>44588</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -5226,16 +5922,16 @@
       <c r="D26" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <v>44589</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>44603</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="27">
         <v>44607</v>
       </c>
       <c r="I26" s="2" t="s">
@@ -5259,16 +5955,16 @@
       <c r="D27" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <v>44589</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>44603</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="27">
         <v>44607</v>
       </c>
       <c r="I27" s="2" t="s">
@@ -5292,16 +5988,16 @@
       <c r="D28" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>44589</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>44603</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="27">
         <v>44607</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -5322,19 +6018,19 @@
       <c r="C29" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <v>44589</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <v>44603</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="27">
         <v>44607</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -5358,16 +6054,16 @@
       <c r="D30" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>44589</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <v>44603</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="27">
         <v>44607</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -5391,16 +6087,16 @@
       <c r="D31" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="12">
         <v>44589</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>44603</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="27">
         <v>44607</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -5424,16 +6120,16 @@
       <c r="D32" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <v>44589</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>44603</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="27">
         <v>44607</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -5457,16 +6153,16 @@
       <c r="D33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="12">
         <v>44589</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>44603</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="27">
         <v>44607</v>
       </c>
       <c r="I33" s="2" t="s">
@@ -5490,16 +6186,16 @@
       <c r="D34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="12">
         <v>44589</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <v>44603</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="27">
         <v>44607</v>
       </c>
       <c r="I34" s="2" t="s">
@@ -5523,16 +6219,16 @@
       <c r="D35" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="12">
         <v>44589</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>44603</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="27">
         <v>44607</v>
       </c>
       <c r="I35" s="2" t="s">
@@ -5556,16 +6252,16 @@
       <c r="D36" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="12">
         <v>44589</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>44603</v>
       </c>
-      <c r="H36" s="11">
+      <c r="H36" s="27">
         <v>44607</v>
       </c>
       <c r="I36" s="2" t="s">
@@ -5589,16 +6285,16 @@
       <c r="D37" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="12">
         <v>44589</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>44603</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="27">
         <v>44607</v>
       </c>
       <c r="I37" s="2" t="s">
@@ -5622,16 +6318,16 @@
       <c r="D38" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="12">
         <v>44589</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="12">
         <v>44603</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="27">
         <v>44607</v>
       </c>
       <c r="I38" s="2" t="s">
@@ -5655,16 +6351,16 @@
       <c r="D39" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="12">
         <v>44589</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G39" s="20">
+      <c r="G39" s="17">
         <v>44603</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="27">
         <v>44607</v>
       </c>
       <c r="I39" s="2" t="s">
@@ -5688,16 +6384,16 @@
       <c r="D40" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="12">
         <v>44589</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="18">
         <v>44603</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="27">
         <v>44607</v>
       </c>
       <c r="I40" s="2" t="s">
@@ -5721,16 +6417,16 @@
       <c r="D41" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="12">
         <v>44589</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="12">
         <v>44603</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="27">
         <v>44607</v>
       </c>
       <c r="I41" s="2" t="s">
@@ -5754,16 +6450,16 @@
       <c r="D42" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="12">
         <v>44589</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="G42" s="21">
+      <c r="G42" s="18">
         <v>44603</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="27">
         <v>44607</v>
       </c>
       <c r="I42" s="2" t="s">
@@ -5787,16 +6483,16 @@
       <c r="D43" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="12">
         <v>44589</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="12">
         <v>44603</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="27">
         <v>44607</v>
       </c>
       <c r="I43" s="2" t="s">
@@ -5820,16 +6516,16 @@
       <c r="D44" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="12">
         <v>44589</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="12">
         <v>44603</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="27">
         <v>44607</v>
       </c>
       <c r="I44" s="2" t="s">
@@ -5853,16 +6549,16 @@
       <c r="D45" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="G45" s="13">
+      <c r="G45" s="12">
         <v>44607</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="27">
         <v>44608</v>
       </c>
       <c r="I45" s="2" t="s">
@@ -5886,16 +6582,16 @@
       <c r="D46" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E46" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="12">
         <v>44607</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="27">
         <v>44608</v>
       </c>
       <c r="I46" s="2" t="s">
@@ -5919,16 +6615,16 @@
       <c r="D47" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="12">
         <v>44607</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="27">
         <v>44608</v>
       </c>
       <c r="I47" s="2" t="s">
@@ -5952,16 +6648,16 @@
       <c r="D48" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G48" s="13">
+      <c r="G48" s="12">
         <v>44607</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="27">
         <v>44601</v>
       </c>
       <c r="I48" s="2" t="s">
@@ -5985,16 +6681,16 @@
       <c r="D49" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="12">
         <v>44607</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="27">
         <v>44606</v>
       </c>
       <c r="I49" s="2" t="s">
@@ -6020,16 +6716,16 @@
       <c r="D50" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E50" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="12">
         <v>44607</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H50" s="27">
         <v>44603</v>
       </c>
       <c r="I50" s="2" t="s">
@@ -6053,16 +6749,16 @@
       <c r="D51" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="12">
         <v>44607</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H51" s="27">
         <v>44603</v>
       </c>
       <c r="I51" s="2" t="s">
@@ -6088,16 +6784,16 @@
       <c r="D52" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G52" s="13">
+      <c r="G52" s="12">
         <v>44607</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H52" s="27">
         <v>44603</v>
       </c>
       <c r="I52" s="2" t="s">
@@ -6123,16 +6819,16 @@
       <c r="D53" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="12">
         <v>44607</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H53" s="27">
         <v>44603</v>
       </c>
       <c r="I53" s="2" t="s">
@@ -6156,16 +6852,16 @@
       <c r="D54" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="13">
+      <c r="G54" s="12">
         <v>44607</v>
       </c>
-      <c r="H54" s="11">
+      <c r="H54" s="27">
         <v>44603</v>
       </c>
       <c r="I54" s="2" t="s">
@@ -6191,16 +6887,16 @@
       <c r="D55" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G55" s="13">
+      <c r="G55" s="12">
         <v>44607</v>
       </c>
-      <c r="H55" s="11">
+      <c r="H55" s="27">
         <v>44607</v>
       </c>
       <c r="I55" s="2" t="s">
@@ -6224,16 +6920,16 @@
       <c r="D56" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E56" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G56" s="13">
+      <c r="G56" s="12">
         <v>44607</v>
       </c>
-      <c r="H56" s="11">
+      <c r="H56" s="27">
         <v>44603</v>
       </c>
       <c r="I56" s="2" t="s">
@@ -6257,16 +6953,16 @@
       <c r="D57" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E57" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="12">
         <v>44607</v>
       </c>
-      <c r="H57" s="11">
+      <c r="H57" s="27">
         <v>44606</v>
       </c>
       <c r="I57" s="2" t="s">
@@ -6290,16 +6986,16 @@
       <c r="D58" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="12">
         <v>44607</v>
       </c>
-      <c r="H58" s="11">
+      <c r="H58" s="27">
         <v>44606</v>
       </c>
       <c r="I58" s="2" t="s">
@@ -6323,16 +7019,16 @@
       <c r="D59" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G59" s="13">
+      <c r="G59" s="12">
         <v>44607</v>
       </c>
-      <c r="H59" s="11">
+      <c r="H59" s="27">
         <v>44606</v>
       </c>
       <c r="I59" s="2" t="s">
@@ -6356,16 +7052,16 @@
       <c r="D60" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E60" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G60" s="13">
+      <c r="G60" s="12">
         <v>44607</v>
       </c>
-      <c r="H60" s="11">
+      <c r="H60" s="27">
         <v>44606</v>
       </c>
       <c r="I60" s="2" t="s">
@@ -6389,16 +7085,16 @@
       <c r="D61" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G61" s="13">
+      <c r="G61" s="12">
         <v>44607</v>
       </c>
-      <c r="H61" s="11">
+      <c r="H61" s="27">
         <v>44603</v>
       </c>
       <c r="I61" s="2" t="s">
@@ -6424,16 +7120,16 @@
       <c r="D62" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E62" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="12">
         <v>44607</v>
       </c>
-      <c r="H62" s="11">
+      <c r="H62" s="27">
         <v>44602</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -6457,16 +7153,16 @@
       <c r="D63" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="12">
         <v>44607</v>
       </c>
-      <c r="H63" s="11">
+      <c r="H63" s="27">
         <v>44608</v>
       </c>
       <c r="I63" s="2" t="s">
@@ -6490,16 +7186,16 @@
       <c r="D64" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E64" s="13" t="s">
+      <c r="E64" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="12">
         <v>44607</v>
       </c>
-      <c r="H64" s="11">
+      <c r="H64" s="27">
         <v>44601</v>
       </c>
       <c r="I64" s="2" t="s">
@@ -6523,16 +7219,16 @@
       <c r="D65" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E65" s="13" t="s">
+      <c r="E65" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="12">
         <v>44607</v>
       </c>
-      <c r="H65" s="11">
+      <c r="H65" s="27">
         <v>44601</v>
       </c>
       <c r="I65" s="2" t="s">
@@ -6556,16 +7252,16 @@
       <c r="D66" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="E66" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="12">
         <v>44607</v>
       </c>
-      <c r="H66" s="11">
+      <c r="H66" s="27">
         <v>44603</v>
       </c>
       <c r="I66" s="2" t="s">
@@ -6589,16 +7285,16 @@
       <c r="D67" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E67" s="12" t="s">
         <v>138</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="12">
         <v>44617</v>
       </c>
-      <c r="H67" s="11">
+      <c r="H67" s="27">
         <v>44608</v>
       </c>
       <c r="I67" s="2" t="s">
@@ -6622,16 +7318,16 @@
       <c r="D68" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="12">
         <v>44615</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G68" s="14">
+      <c r="G68" s="13">
         <v>44642</v>
       </c>
-      <c r="H68" s="11">
+      <c r="H68" s="27">
         <v>44642</v>
       </c>
       <c r="I68" s="2" t="s">
@@ -6653,16 +7349,16 @@
       <c r="D69" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E69" s="13">
+      <c r="E69" s="12">
         <v>44615</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G69" s="14">
+      <c r="G69" s="13">
         <v>44631</v>
       </c>
-      <c r="H69" s="14">
+      <c r="H69" s="27">
         <v>44631</v>
       </c>
       <c r="I69" s="2" t="s">
@@ -6686,16 +7382,16 @@
       <c r="D70" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E70" s="13">
+      <c r="E70" s="12">
         <v>44615</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G70" s="14">
+      <c r="G70" s="13">
         <v>44631</v>
       </c>
-      <c r="H70" s="14">
+      <c r="H70" s="27">
         <v>44631</v>
       </c>
       <c r="I70" s="2" t="s">
@@ -6719,16 +7415,16 @@
       <c r="D71" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E71" s="13">
+      <c r="E71" s="12">
         <v>44615</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G71" s="14">
+      <c r="G71" s="13">
         <v>44635</v>
       </c>
-      <c r="H71" s="14">
+      <c r="H71" s="27">
         <v>44635</v>
       </c>
       <c r="I71" s="2" t="s">
@@ -6752,16 +7448,16 @@
       <c r="D72" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E72" s="13">
+      <c r="E72" s="12">
         <v>44615</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G72" s="14">
+      <c r="G72" s="13">
         <v>44631</v>
       </c>
-      <c r="H72" s="14">
+      <c r="H72" s="27">
         <v>44631</v>
       </c>
       <c r="I72" s="2" t="s">
@@ -6785,16 +7481,16 @@
       <c r="D73" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E73" s="13">
+      <c r="E73" s="12">
         <v>44615</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G73" s="14">
+      <c r="G73" s="13">
         <v>44635</v>
       </c>
-      <c r="H73" s="14">
+      <c r="H73" s="27">
         <v>44635</v>
       </c>
       <c r="I73" s="2" t="s">
@@ -6818,16 +7514,16 @@
       <c r="D74" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E74" s="13">
+      <c r="E74" s="12">
         <v>44615</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="G74" s="14">
+      <c r="G74" s="13">
         <v>44635</v>
       </c>
-      <c r="H74" s="14">
+      <c r="H74" s="27">
         <v>44635</v>
       </c>
       <c r="I74" s="2" t="s">
@@ -6851,16 +7547,16 @@
       <c r="D75" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E75" s="13">
+      <c r="E75" s="12">
         <v>44615</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="13">
         <v>44636</v>
       </c>
-      <c r="H75" s="11">
+      <c r="H75" s="27">
         <v>44634</v>
       </c>
       <c r="I75" s="2" t="s">
@@ -6884,16 +7580,16 @@
       <c r="D76" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E76" s="13">
+      <c r="E76" s="12">
         <v>44615</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G76" s="14">
+      <c r="G76" s="13">
         <v>44636</v>
       </c>
-      <c r="H76" s="11">
+      <c r="H76" s="27">
         <v>44634</v>
       </c>
       <c r="I76" s="2" t="s">
@@ -6917,16 +7613,16 @@
       <c r="D77" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E77" s="13">
+      <c r="E77" s="12">
         <v>44615</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G77" s="14">
+      <c r="G77" s="13">
         <v>44636</v>
       </c>
-      <c r="H77" s="11">
+      <c r="H77" s="27">
         <v>44634</v>
       </c>
       <c r="I77" s="2" t="s">
@@ -6950,16 +7646,16 @@
       <c r="D78" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E78" s="13">
+      <c r="E78" s="12">
         <v>44615</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G78" s="14">
+      <c r="G78" s="13">
         <v>44636</v>
       </c>
-      <c r="H78" s="11">
+      <c r="H78" s="27">
         <v>44634</v>
       </c>
       <c r="I78" s="2" t="s">
@@ -6983,16 +7679,16 @@
       <c r="D79" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E79" s="13">
+      <c r="E79" s="12">
         <v>44615</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="G79" s="14">
+      <c r="G79" s="13">
         <v>44636</v>
       </c>
-      <c r="H79" s="11">
+      <c r="H79" s="27">
         <v>44634</v>
       </c>
       <c r="I79" s="2" t="s">
@@ -7016,16 +7712,16 @@
       <c r="D80" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E80" s="13">
+      <c r="E80" s="12">
         <v>44615</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="G80" s="14">
+      <c r="G80" s="13">
         <v>44636</v>
       </c>
-      <c r="H80" s="11">
+      <c r="H80" s="27">
         <v>44634</v>
       </c>
       <c r="I80" s="2" t="s">
@@ -7049,16 +7745,16 @@
       <c r="D81" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E81" s="13">
+      <c r="E81" s="12">
         <v>44615</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G81" s="14">
+      <c r="G81" s="13">
         <v>44636</v>
       </c>
-      <c r="H81" s="11">
+      <c r="H81" s="27">
         <v>44634</v>
       </c>
       <c r="I81" s="2" t="s">
@@ -7079,19 +7775,19 @@
       <c r="C82" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="D82" s="23" t="s">
+      <c r="D82" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="E82" s="13">
+      <c r="E82" s="12">
         <v>44615</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G82" s="14">
+      <c r="G82" s="13">
         <v>44636</v>
       </c>
-      <c r="H82" s="11">
+      <c r="H82" s="27">
         <v>44634</v>
       </c>
       <c r="I82" s="2" t="s">
@@ -7115,16 +7811,16 @@
       <c r="D83" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E83" s="13">
+      <c r="E83" s="12">
         <v>44615</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G83" s="14">
+      <c r="G83" s="13">
         <v>44636</v>
       </c>
-      <c r="H83" s="11">
+      <c r="H83" s="27">
         <v>44634</v>
       </c>
       <c r="I83" s="2" t="s">
@@ -7145,19 +7841,19 @@
       <c r="C84" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D84" s="35" t="s">
+      <c r="D84" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="E84" s="36">
+      <c r="E84" s="23">
         <v>44635</v>
       </c>
-      <c r="F84" s="37" t="s">
+      <c r="F84" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="G84" s="14">
+      <c r="G84" s="13">
         <v>44649</v>
       </c>
-      <c r="H84" s="14">
+      <c r="H84" s="27">
         <v>44649</v>
       </c>
       <c r="I84" s="2" t="s">
@@ -7179,16 +7875,16 @@
       <c r="D85" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E85" s="13">
+      <c r="E85" s="12">
         <v>44635</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="G85" s="14">
+      <c r="G85" s="13">
         <v>44643</v>
       </c>
-      <c r="H85" s="11">
+      <c r="H85" s="27">
         <v>44642</v>
       </c>
       <c r="I85" s="2" t="s">
@@ -7207,19 +7903,19 @@
       <c r="C86" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D86" s="35" t="s">
+      <c r="D86" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="E86" s="36">
+      <c r="E86" s="23">
         <v>44635</v>
       </c>
-      <c r="F86" s="37" t="s">
+      <c r="F86" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="G86" s="14">
+      <c r="G86" s="13">
         <v>44649</v>
       </c>
-      <c r="H86" s="14">
+      <c r="H86" s="27">
         <v>44649</v>
       </c>
       <c r="I86" s="2" t="s">
@@ -7241,16 +7937,16 @@
       <c r="D87" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E87" s="13">
+      <c r="E87" s="12">
         <v>44635</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G87" s="14">
+      <c r="G87" s="13">
         <v>44643</v>
       </c>
-      <c r="H87" s="11">
+      <c r="H87" s="27">
         <v>44642</v>
       </c>
       <c r="I87" s="2" t="s">
@@ -7269,20 +7965,24 @@
       <c r="C88" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D88" s="35" t="s">
+      <c r="D88" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E88" s="36">
+      <c r="E88" s="23">
         <v>44635</v>
       </c>
-      <c r="F88" s="37" t="s">
+      <c r="F88" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="G88" s="14">
+      <c r="G88" s="13">
         <v>44649</v>
       </c>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
+      <c r="H88" s="27">
+        <v>44649</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
@@ -7296,19 +7996,19 @@
       <c r="C89" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="35" t="s">
+      <c r="D89" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="E89" s="36">
+      <c r="E89" s="23">
         <v>44635</v>
       </c>
-      <c r="F89" s="37" t="s">
+      <c r="F89" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="G89" s="14">
+      <c r="G89" s="13">
         <v>44641</v>
       </c>
-      <c r="H89" s="11">
+      <c r="H89" s="27">
         <v>44642</v>
       </c>
       <c r="I89" s="2" t="s">
@@ -7330,16 +8030,16 @@
       <c r="D90" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E90" s="13">
+      <c r="E90" s="12">
         <v>44635</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="G90" s="14">
+      <c r="G90" s="13">
         <v>44641</v>
       </c>
-      <c r="H90" s="11">
+      <c r="H90" s="27">
         <v>44642</v>
       </c>
       <c r="I90" s="2" t="s">
@@ -7358,19 +8058,19 @@
       <c r="C91" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="D91" s="35" t="s">
+      <c r="D91" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="E91" s="36">
+      <c r="E91" s="23">
         <v>44635</v>
       </c>
-      <c r="F91" s="37" t="s">
+      <c r="F91" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="G91" s="14">
+      <c r="G91" s="13">
         <v>44645</v>
       </c>
-      <c r="H91" s="11">
+      <c r="H91" s="27">
         <v>44648</v>
       </c>
       <c r="I91" s="2" t="s">
@@ -7392,16 +8092,16 @@
       <c r="D92" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E92" s="13">
+      <c r="E92" s="12">
         <v>44635</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G92" s="14">
+      <c r="G92" s="13">
         <v>44641</v>
       </c>
-      <c r="H92" s="11">
+      <c r="H92" s="27">
         <v>44642</v>
       </c>
       <c r="I92" s="2" t="s">
@@ -7423,16 +8123,16 @@
       <c r="D93" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="E93" s="13">
+      <c r="E93" s="12">
         <v>44638</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="G93" s="14">
+      <c r="G93" s="13">
         <v>44642</v>
       </c>
-      <c r="H93" s="11">
+      <c r="H93" s="27">
         <v>44641</v>
       </c>
       <c r="I93" s="2" t="s">
@@ -7454,13 +8154,21 @@
       <c r="D94" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="E94" s="13">
+      <c r="E94" s="12">
         <v>44649</v>
       </c>
-      <c r="F94" s="2"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
+      <c r="F94" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="G94" s="13">
+        <v>44650</v>
+      </c>
+      <c r="H94" s="27">
+        <v>44650</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
@@ -7477,20 +8185,47 @@
       <c r="D95" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="E95" s="13">
+      <c r="E95" s="12">
         <v>44649</v>
       </c>
       <c r="F95" s="2"/>
-      <c r="G95" s="14">
+      <c r="G95" s="13">
         <v>44651</v>
       </c>
-      <c r="H95" s="2"/>
+      <c r="H95" s="28"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
+    <row r="96" spans="1:11" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B96" s="2">
+        <v>3</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E96" s="12">
+        <v>44649</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="G96" s="13">
+        <v>44651</v>
+      </c>
+      <c r="H96" s="28"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K93" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K96" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7547,1191 +8282,1333 @@
         <oleObject progId="封裝程式殼層物件" shapeId="1026" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Worksheet" shapeId="1029" r:id="rId8">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId9">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>2720340</xdr:colOff>
+                <xdr:row>95</xdr:row>
+                <xdr:rowOff>632460</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>3009900</xdr:colOff>
+                <xdr:row>95</xdr:row>
+                <xdr:rowOff>906780</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Worksheet" shapeId="1029" r:id="rId8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E69748B-F013-4C3D-B545-0E0A517A1BB7}">
-  <dimension ref="A3:T25"/>
+  <dimension ref="A3:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12" style="34" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.77734375" style="34"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="40" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="34" t="s">
         <v>238</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="34" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="34" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42">
         <v>22</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="42">
         <v>22</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="42">
         <v>1</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="42">
         <v>1</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28">
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42">
         <v>23</v>
       </c>
-      <c r="S6" s="28">
+      <c r="S6" s="42">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
+      <c r="A7" s="43">
         <v>44575</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="42">
         <v>21</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="42">
         <v>21</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28">
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42">
         <v>21</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7" s="42">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+      <c r="A8" s="43">
         <v>44587</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42">
         <v>3</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="42">
         <v>3</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28">
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42">
         <v>3</v>
       </c>
-      <c r="S8" s="28">
+      <c r="S8" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+      <c r="A9" s="43">
         <v>44589</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28">
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42">
         <v>19</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="42">
         <v>19</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28">
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42">
         <v>19</v>
       </c>
-      <c r="S9" s="28">
+      <c r="S9" s="42">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+      <c r="A10" s="43">
         <v>44615</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42">
         <v>3</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="42">
         <v>3</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="42">
         <v>12</v>
       </c>
-      <c r="M10" s="28">
+      <c r="M10" s="42">
         <v>12</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="42">
         <v>1</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="42">
         <v>1</v>
       </c>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28">
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42">
         <v>16</v>
       </c>
-      <c r="S10" s="28">
+      <c r="S10" s="42">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="29">
+      <c r="A11" s="43">
         <v>44635</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28">
-        <v>7</v>
-      </c>
-      <c r="O11" s="28">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42">
         <v>6</v>
       </c>
-      <c r="P11" s="28">
+      <c r="O11" s="42">
+        <v>6</v>
+      </c>
+      <c r="P11" s="42">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="42">
+        <v>3</v>
+      </c>
+      <c r="R11" s="42">
+        <v>9</v>
+      </c>
+      <c r="S11" s="42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="43">
+        <v>44638</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42">
+        <v>1</v>
+      </c>
+      <c r="O12" s="42">
+        <v>1</v>
+      </c>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42">
+        <v>1</v>
+      </c>
+      <c r="S12" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="43">
+        <v>44649</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42">
         <v>2</v>
       </c>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28">
-        <v>9</v>
-      </c>
-      <c r="S11" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="29">
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42">
+        <v>2</v>
+      </c>
+      <c r="S13" s="42"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="42">
+        <v>21</v>
+      </c>
+      <c r="C14" s="42">
+        <v>21</v>
+      </c>
+      <c r="D14" s="42">
+        <v>22</v>
+      </c>
+      <c r="E14" s="42">
+        <v>22</v>
+      </c>
+      <c r="F14" s="42">
+        <v>22</v>
+      </c>
+      <c r="G14" s="42">
+        <v>22</v>
+      </c>
+      <c r="H14" s="42">
+        <v>1</v>
+      </c>
+      <c r="I14" s="42">
+        <v>1</v>
+      </c>
+      <c r="J14" s="42">
+        <v>3</v>
+      </c>
+      <c r="K14" s="42">
+        <v>3</v>
+      </c>
+      <c r="L14" s="42">
+        <v>12</v>
+      </c>
+      <c r="M14" s="42">
+        <v>12</v>
+      </c>
+      <c r="N14" s="42">
+        <v>8</v>
+      </c>
+      <c r="O14" s="42">
+        <v>8</v>
+      </c>
+      <c r="P14" s="42">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="42">
+        <v>3</v>
+      </c>
+      <c r="R14" s="42">
+        <v>94</v>
+      </c>
+      <c r="S14" s="42">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="30">
+        <v>44583</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30">
+        <v>44603</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30">
+        <v>44610</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30">
+        <v>44617</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30">
+        <v>44631</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30">
         <v>44638</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28">
-        <v>1</v>
-      </c>
-      <c r="O12" s="28">
-        <v>1</v>
-      </c>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28">
-        <v>1</v>
-      </c>
-      <c r="S12" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="B13" s="28">
-        <v>21</v>
-      </c>
-      <c r="C13" s="28">
-        <v>21</v>
-      </c>
-      <c r="D13" s="28">
-        <v>22</v>
-      </c>
-      <c r="E13" s="28">
-        <v>22</v>
-      </c>
-      <c r="F13" s="28">
-        <v>22</v>
-      </c>
-      <c r="G13" s="28">
-        <v>22</v>
-      </c>
-      <c r="H13" s="28">
-        <v>1</v>
-      </c>
-      <c r="I13" s="28">
-        <v>1</v>
-      </c>
-      <c r="J13" s="28">
-        <v>3</v>
-      </c>
-      <c r="K13" s="28">
-        <v>3</v>
-      </c>
-      <c r="L13" s="28">
-        <v>12</v>
-      </c>
-      <c r="M13" s="28">
-        <v>12</v>
-      </c>
-      <c r="N13" s="28">
-        <v>9</v>
-      </c>
-      <c r="O13" s="28">
-        <v>8</v>
-      </c>
-      <c r="P13" s="28">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28">
-        <v>92</v>
-      </c>
-      <c r="S13" s="28">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="B16" s="33">
-        <v>44583</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33">
-        <v>44603</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33">
-        <v>44610</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33">
-        <v>44617</v>
-      </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33">
-        <v>44631</v>
-      </c>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33">
-        <v>44638</v>
-      </c>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33">
+      <c r="M16" s="30"/>
+      <c r="N16" s="30">
         <v>44645</v>
       </c>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33">
+      <c r="O16" s="30"/>
+      <c r="P16" s="30">
         <v>44651</v>
       </c>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="32" t="s">
+      <c r="Q16" s="30"/>
+      <c r="R16" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="B17" s="34" t="str">
+      <c r="B17" s="32" t="str">
         <f t="shared" ref="B17:Q17" si="0">B5</f>
         <v>預計</v>
       </c>
-      <c r="C17" s="34" t="str">
+      <c r="C17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="D17" s="34" t="str">
+      <c r="D17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="E17" s="34" t="str">
+      <c r="E17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="F17" s="34" t="str">
+      <c r="F17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="G17" s="34" t="str">
+      <c r="G17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="H17" s="34" t="str">
+      <c r="H17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="I17" s="34" t="str">
+      <c r="I17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="J17" s="34" t="str">
+      <c r="J17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="K17" s="34" t="str">
+      <c r="K17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="L17" s="34" t="str">
+      <c r="L17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="M17" s="34" t="str">
+      <c r="M17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="N17" s="34" t="str">
+      <c r="N17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="O17" s="34" t="str">
+      <c r="O17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="P17" s="34" t="str">
+      <c r="P17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>預計</v>
       </c>
-      <c r="Q17" s="34" t="str">
+      <c r="Q17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>實際</v>
       </c>
-      <c r="R17" s="18" t="s">
+      <c r="R17" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="S17" s="18" t="s">
+      <c r="S17" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="T17" s="18" t="s">
+      <c r="T17" s="33" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="str">
+      <c r="A18" s="25" t="str">
         <f t="shared" ref="A18:S18" si="1">A6</f>
         <v>2022/2/8、2022/2/11</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="34">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="34">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="34">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="34">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="17">
+      <c r="N18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="17">
+      <c r="O18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P18" s="17">
+      <c r="P18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R18" s="18">
+      <c r="R18" s="33">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="S18" s="18">
+      <c r="S18" s="33">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="T18" s="25">
+      <c r="T18" s="35">
         <f>S18/R18</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="31">
+      <c r="A19" s="36">
         <f t="shared" ref="A19:S19" si="2">A7</f>
         <v>44575</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="34">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="34">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O19" s="17">
+      <c r="O19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P19" s="17">
+      <c r="P19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="17">
+      <c r="Q19" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R19" s="18">
+      <c r="R19" s="33">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="S19" s="18">
+      <c r="S19" s="33">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="T19" s="25">
-        <f t="shared" ref="T19:T25" si="3">S19/R19</f>
+      <c r="T19" s="35">
+        <f t="shared" ref="T19:T23" si="3">S19/R19</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="31">
+      <c r="A20" s="36">
         <f t="shared" ref="A20:S20" si="4">A8</f>
         <v>44587</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="34">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="34">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L20" s="17">
+      <c r="L20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P20" s="17">
+      <c r="P20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="17">
+      <c r="Q20" s="34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R20" s="18">
+      <c r="R20" s="33">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="S20" s="18">
+      <c r="S20" s="33">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="T20" s="25">
+      <c r="T20" s="35">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="31">
+      <c r="A21" s="36">
         <f t="shared" ref="A21:S21" si="5">A9</f>
         <v>44589</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="34">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="34">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K21" s="17">
+      <c r="K21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P21" s="17">
+      <c r="P21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R21" s="18">
+      <c r="R21" s="33">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="S21" s="18">
+      <c r="S21" s="33">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="T21" s="25">
+      <c r="T21" s="35">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="31">
+      <c r="A22" s="36">
         <f t="shared" ref="A22:S22" si="6">A10</f>
         <v>44615</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="34">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="K22" s="17">
+      <c r="K22" s="34">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="L22" s="17">
+      <c r="L22" s="34">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="M22" s="17">
+      <c r="M22" s="34">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="N22" s="17">
+      <c r="N22" s="34">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O22" s="17">
+      <c r="O22" s="34">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P22" s="17">
+      <c r="P22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="17">
+      <c r="Q22" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R22" s="18">
+      <c r="R22" s="33">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="S22" s="18">
+      <c r="S22" s="33">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="T22" s="25">
+      <c r="T22" s="35">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="31">
+      <c r="A23" s="36">
         <f t="shared" ref="A23:S23" si="7">A11</f>
         <v>44635</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K23" s="17">
+      <c r="K23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L23" s="17">
+      <c r="L23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M23" s="17">
+      <c r="M23" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N23" s="17">
-        <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="O23" s="17">
+      <c r="N23" s="34">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="P23" s="17">
+      <c r="O23" s="34">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="Q23" s="17">
+        <v>6</v>
+      </c>
+      <c r="P23" s="34">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="18">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="34">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="R23" s="33">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="S23" s="18">
+      <c r="S23" s="33">
         <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="T23" s="25">
+        <v>9</v>
+      </c>
+      <c r="T23" s="35">
         <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="31">
+      <c r="A24" s="36">
         <f t="shared" ref="A24:S24" si="8">A12</f>
         <v>44638</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I24" s="17">
+      <c r="I24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K24" s="17">
+      <c r="K24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L24" s="17">
+      <c r="L24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M24" s="17">
+      <c r="M24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N24" s="17">
+      <c r="N24" s="34">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="O24" s="17">
+      <c r="O24" s="34">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P24" s="17">
+      <c r="P24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="17">
+      <c r="Q24" s="34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="R24" s="18">
+      <c r="R24" s="33">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="S24" s="18">
+      <c r="S24" s="33">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="T24" s="25"/>
+      <c r="T24" s="35">
+        <f t="shared" ref="T24:T26" si="9">S24/R24</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="34" t="str">
-        <f t="shared" ref="A25:S25" si="9">A13</f>
+      <c r="A25" s="36">
+        <f t="shared" ref="A25:S25" si="10">A13</f>
+        <v>44649</v>
+      </c>
+      <c r="B25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="34">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="Q25" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="33">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="S25" s="33">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="37" t="str">
+        <f t="shared" ref="A26:S26" si="11">A14</f>
         <v>總計</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B26" s="32">
+        <f t="shared" si="11"/>
+        <v>21</v>
+      </c>
+      <c r="C26" s="32">
+        <f t="shared" si="11"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="32">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="E26" s="32">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="F26" s="32">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="G26" s="32">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="H26" s="32">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="32">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="J26" s="32">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="K26" s="32">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="L26" s="32">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="M26" s="32">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="N26" s="32">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="O26" s="32">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="P26" s="32">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="Q26" s="32">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="R26" s="38">
+        <f t="shared" si="11"/>
+        <v>94</v>
+      </c>
+      <c r="S26" s="38">
+        <f t="shared" si="11"/>
+        <v>92</v>
+      </c>
+      <c r="T26" s="39">
         <f t="shared" si="9"/>
-        <v>21</v>
-      </c>
-      <c r="C25" s="34">
-        <f t="shared" si="9"/>
-        <v>21</v>
-      </c>
-      <c r="D25" s="34">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="E25" s="34">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="F25" s="34">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="G25" s="34">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="H25" s="34">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="34">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="J25" s="34">
-        <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="K25" s="34">
-        <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="L25" s="34">
-        <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-      <c r="M25" s="34">
-        <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-      <c r="N25" s="34">
-        <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="O25" s="34">
-        <f t="shared" si="9"/>
-        <v>8</v>
-      </c>
-      <c r="P25" s="34">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="Q25" s="34">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="18">
-        <f t="shared" si="9"/>
-        <v>92</v>
-      </c>
-      <c r="S25" s="18">
-        <f t="shared" si="9"/>
-        <v>89</v>
-      </c>
-      <c r="T25" s="25">
-        <f t="shared" si="3"/>
-        <v>0.96739130434782605</v>
+        <v>0.97872340425531912</v>
       </c>
     </row>
   </sheetData>
@@ -8742,6 +9619,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -8855,33 +9747,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8902,9 +9771,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/04/08 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS交付區/回覆SKL反應問題/簡易審查紀錄表User意見彙總回覆.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\需求規格書\0.審查意見與回覆\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.16\St1Share(NAS)\SKL\需求規格書\0.審查意見與回覆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86003A20-F262-453C-9DB7-DFD82E53EE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE345F1-51B1-445D-A7D8-03FEAE6D3C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11390C71-8784-468D-A357-EFCA9ACACA98}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="270">
   <si>
     <t>章節及說明</t>
   </si>
@@ -5078,13 +5078,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I96" sqref="I96"/>
+      <selection pane="bottomLeft" activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5138,7 +5137,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -5171,7 +5170,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -5204,7 +5203,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -5237,7 +5236,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -5270,7 +5269,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -5303,7 +5302,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -5336,7 +5335,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -5369,7 +5368,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -5402,7 +5401,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -5435,7 +5434,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -5468,7 +5467,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="105" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -5501,7 +5500,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -5534,7 +5533,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -5567,7 +5566,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -5600,7 +5599,7 @@
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -5633,7 +5632,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -5666,7 +5665,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -5699,7 +5698,7 @@
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -5732,7 +5731,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -5765,7 +5764,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -5798,7 +5797,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -5831,7 +5830,7 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5864,7 +5863,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="285" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="285" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -5897,7 +5896,7 @@
       </c>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -5930,7 +5929,7 @@
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="225" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -5963,7 +5962,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -5996,7 +5995,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -6029,7 +6028,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -6062,7 +6061,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -6095,7 +6094,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -6128,7 +6127,7 @@
       </c>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="90" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="90" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -6161,7 +6160,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -6194,7 +6193,7 @@
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -6227,7 +6226,7 @@
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -6260,7 +6259,7 @@
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>74</v>
       </c>
@@ -6293,7 +6292,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="105" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -6326,7 +6325,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -6359,7 +6358,7 @@
       </c>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -6392,7 +6391,7 @@
       </c>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
@@ -6425,7 +6424,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -6458,7 +6457,7 @@
       </c>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="180" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
@@ -6491,7 +6490,7 @@
       </c>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
@@ -6524,7 +6523,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -6557,7 +6556,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="345" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="345" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -6590,7 +6589,7 @@
       </c>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -6623,7 +6622,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="120" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -6656,7 +6655,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -6689,7 +6688,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -6724,7 +6723,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -6757,7 +6756,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -6792,7 +6791,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -6827,7 +6826,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -6860,7 +6859,7 @@
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -6895,7 +6894,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -6928,7 +6927,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -6961,7 +6960,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -6994,7 +6993,7 @@
       </c>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -7027,7 +7026,7 @@
       </c>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -7060,7 +7059,7 @@
       </c>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -7093,7 +7092,7 @@
       </c>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -7128,7 +7127,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -7161,7 +7160,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -7194,7 +7193,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -7227,7 +7226,7 @@
       </c>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -7260,7 +7259,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -7293,7 +7292,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="135" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -7326,7 +7325,7 @@
       </c>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>170</v>
       </c>
@@ -7357,7 +7356,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>170</v>
       </c>
@@ -7390,7 +7389,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>170</v>
       </c>
@@ -7423,7 +7422,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>170</v>
       </c>
@@ -7456,7 +7455,7 @@
       </c>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>170</v>
       </c>
@@ -7489,7 +7488,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -7522,7 +7521,7 @@
       </c>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>170</v>
       </c>
@@ -7555,7 +7554,7 @@
       </c>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>170</v>
       </c>
@@ -7588,7 +7587,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -7621,7 +7620,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>170</v>
       </c>
@@ -7654,7 +7653,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -7687,7 +7686,7 @@
       </c>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>170</v>
       </c>
@@ -7720,7 +7719,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>170</v>
       </c>
@@ -7753,7 +7752,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>170</v>
       </c>
@@ -7786,7 +7785,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>170</v>
       </c>
@@ -7819,7 +7818,7 @@
       </c>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>170</v>
       </c>
@@ -7852,7 +7851,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>170</v>
       </c>
@@ -7883,7 +7882,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>170</v>
       </c>
@@ -7914,7 +7913,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -7945,7 +7944,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -7976,7 +7975,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -8007,7 +8006,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>170</v>
       </c>
@@ -8038,7 +8037,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>170</v>
       </c>
@@ -8069,7 +8068,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>170</v>
       </c>
@@ -8100,7 +8099,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>170</v>
       </c>
@@ -8131,7 +8130,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>246</v>
       </c>
@@ -8162,7 +8161,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="150" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>257</v>
       </c>
@@ -8193,7 +8192,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>259</v>
       </c>
@@ -8247,16 +8246,14 @@
       <c r="H96" s="12">
         <v>44658</v>
       </c>
-      <c r="I96" s="2"/>
+      <c r="I96" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K96" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K96" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9762,12 +9759,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100D090CFB557704A4BB37222FC84541896" ma:contentTypeVersion="" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="6da6cad0fb8fa2c72d1cc04d17c9ed5c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d02a0c37e3e6f72aa1a25fa502656a20">
     <xsd:element name="properties">
@@ -9881,6 +9872,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BF9683-E989-4811-AF75-1F48F16EEFFF}">
   <ds:schemaRefs>
@@ -9890,21 +9887,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED3893BD-2957-455B-B4FE-BFC89A307F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9918,4 +9900,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D38D02-28B5-45A1-A88A-7F33649092C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>